<commit_message>
Completed 2 other interval problems
</commit_message>
<xml_diff>
--- a/Leetcode 75.xlsx
+++ b/Leetcode 75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christianm\Desktop\Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC35D622-6A72-4076-AD6C-87BBF8D562B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A21F16A-53A9-4387-A6D1-B1508ACF8684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="318">
   <si>
     <t>Video Solution</t>
   </si>
@@ -985,7 +985,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1088,14 +1088,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1243,7 +1235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1282,9 +1274,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1506,7 +1495,7 @@
   <dimension ref="A1:F1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2248,7 +2237,9 @@
       <c r="B38" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C38" s="18"/>
+      <c r="C38" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="D38" s="10" t="s">
         <v>157</v>
       </c>
@@ -2266,7 +2257,7 @@
       <c r="B39" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="C39" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D39" s="8" t="s">
@@ -2286,7 +2277,9 @@
       <c r="B40" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="C40" s="18"/>
+      <c r="C40" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="D40" s="10" t="s">
         <v>165</v>
       </c>

</xml_diff>

<commit_message>
Completed Valid_Tree.py & updated spreadsheet.
</commit_message>
<xml_diff>
--- a/Leetcode 75.xlsx
+++ b/Leetcode 75.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christianm\Desktop\Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A21F16A-53A9-4387-A6D1-B1508ACF8684}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77E7C27-BCE9-427A-9B4A-E6A545DD4DCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="318">
   <si>
     <t>Video Solution</t>
   </si>
@@ -1494,8 +1494,8 @@
   </sheetPr>
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2163,7 +2163,9 @@
       <c r="B34" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="C34" s="13"/>
+      <c r="C34" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="D34" s="10" t="s">
         <v>140</v>
       </c>

</xml_diff>

<commit_message>
Completed rotate image (matrix) problem
</commit_message>
<xml_diff>
--- a/Leetcode 75.xlsx
+++ b/Leetcode 75.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christianm\Desktop\Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748BC439-83F9-4F6F-ACB1-898A27E949D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D02DC5D-C1CD-4D76-AA9A-A46B3524C0D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="318">
   <si>
     <t>Video Solution</t>
   </si>
@@ -985,7 +985,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1088,6 +1088,14 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1235,7 +1243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1274,6 +1282,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1494,21 +1505,21 @@
   </sheetPr>
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" customWidth="1"/>
-    <col min="4" max="4" width="64.140625" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" customWidth="1"/>
-    <col min="6" max="6" width="182.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.44140625" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" customWidth="1"/>
+    <col min="4" max="4" width="64.109375" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" customWidth="1"/>
+    <col min="6" max="6" width="182.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1528,7 +1539,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -1548,7 +1559,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
@@ -1568,7 +1579,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -1588,7 +1599,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -1608,7 +1619,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -1628,7 +1639,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>28</v>
       </c>
@@ -1648,7 +1659,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
@@ -1668,7 +1679,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>36</v>
       </c>
@@ -1688,7 +1699,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>40</v>
       </c>
@@ -1708,7 +1719,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>44</v>
       </c>
@@ -1728,7 +1739,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>48</v>
       </c>
@@ -1748,7 +1759,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>53</v>
       </c>
@@ -1768,7 +1779,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>57</v>
       </c>
@@ -1786,7 +1797,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>61</v>
       </c>
@@ -1806,7 +1817,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>65</v>
       </c>
@@ -1824,7 +1835,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>69</v>
       </c>
@@ -1844,7 +1855,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>74</v>
       </c>
@@ -1864,7 +1875,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>78</v>
       </c>
@@ -1884,7 +1895,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>82</v>
       </c>
@@ -1904,7 +1915,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>86</v>
       </c>
@@ -1924,7 +1935,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>90</v>
       </c>
@@ -1944,7 +1955,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>94</v>
       </c>
@@ -1964,7 +1975,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>98</v>
       </c>
@@ -1984,7 +1995,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>102</v>
       </c>
@@ -2004,7 +2015,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>106</v>
       </c>
@@ -2024,7 +2035,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>110</v>
       </c>
@@ -2044,7 +2055,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>114</v>
       </c>
@@ -2064,7 +2075,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>119</v>
       </c>
@@ -2082,7 +2093,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>123</v>
       </c>
@@ -2100,7 +2111,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>127</v>
       </c>
@@ -2120,7 +2131,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>131</v>
       </c>
@@ -2138,7 +2149,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16" t="s">
         <v>135</v>
       </c>
@@ -2156,7 +2167,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16" t="s">
         <v>139</v>
       </c>
@@ -2176,7 +2187,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="16" t="s">
         <v>143</v>
       </c>
@@ -2196,7 +2207,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>147</v>
       </c>
@@ -2214,7 +2225,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>152</v>
       </c>
@@ -2232,7 +2243,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>156</v>
       </c>
@@ -2252,7 +2263,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>160</v>
       </c>
@@ -2272,7 +2283,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="19" t="s">
         <v>164</v>
       </c>
@@ -2292,7 +2303,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
         <v>168</v>
       </c>
@@ -2312,7 +2323,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
         <v>173</v>
       </c>
@@ -2332,7 +2343,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>177</v>
       </c>
@@ -2352,7 +2363,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
         <v>181</v>
       </c>
@@ -2372,7 +2383,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
         <v>185</v>
       </c>
@@ -2392,7 +2403,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
         <v>189</v>
       </c>
@@ -2412,7 +2423,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5" t="s">
         <v>193</v>
       </c>
@@ -2430,7 +2441,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
         <v>198</v>
       </c>
@@ -2450,14 +2461,16 @@
         <v>201</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
         <v>202</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="C49" s="18"/>
+      <c r="C49" s="24" t="s">
+        <v>8</v>
+      </c>
       <c r="D49" s="10" t="s">
         <v>203</v>
       </c>
@@ -2468,7 +2481,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
         <v>206</v>
       </c>
@@ -2488,7 +2501,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
         <v>210</v>
       </c>
@@ -2508,7 +2521,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
         <v>215</v>
       </c>
@@ -2528,7 +2541,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="21" t="s">
         <v>219</v>
       </c>
@@ -2548,7 +2561,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
         <v>223</v>
       </c>
@@ -2568,7 +2581,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="5" t="s">
         <v>227</v>
       </c>
@@ -2588,7 +2601,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
         <v>231</v>
       </c>
@@ -2608,7 +2621,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
         <v>235</v>
       </c>
@@ -2628,7 +2641,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
         <v>239</v>
       </c>
@@ -2648,7 +2661,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
         <v>243</v>
       </c>
@@ -2668,7 +2681,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="16" t="s">
         <v>247</v>
       </c>
@@ -2688,7 +2701,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
         <v>251</v>
       </c>
@@ -2708,7 +2721,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
         <v>256</v>
       </c>
@@ -2728,7 +2741,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
         <v>260</v>
       </c>
@@ -2748,7 +2761,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
         <v>264</v>
       </c>
@@ -2766,7 +2779,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="s">
         <v>268</v>
       </c>
@@ -2786,7 +2799,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
         <v>272</v>
       </c>
@@ -2804,7 +2817,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
         <v>276</v>
       </c>
@@ -2824,7 +2837,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
         <v>280</v>
       </c>
@@ -2844,7 +2857,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
         <v>284</v>
       </c>
@@ -2864,7 +2877,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
         <v>288</v>
       </c>
@@ -2884,7 +2897,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
         <v>292</v>
       </c>
@@ -2904,7 +2917,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
         <v>296</v>
       </c>
@@ -2924,7 +2937,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
         <v>300</v>
       </c>
@@ -2944,7 +2957,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
         <v>304</v>
       </c>
@@ -2964,7 +2977,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
         <v>181</v>
       </c>
@@ -2982,7 +2995,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
         <v>310</v>
       </c>
@@ -3000,7 +3013,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="s">
         <v>314</v>
       </c>
@@ -3018,2973 +3031,2973 @@
         <v>317</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C78" s="22"/>
     </row>
-    <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C79" s="22"/>
     </row>
-    <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="23"/>
       <c r="C80" s="22"/>
     </row>
-    <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="23"/>
       <c r="C81" s="22"/>
     </row>
-    <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="23"/>
       <c r="C82" s="22"/>
     </row>
-    <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="23"/>
       <c r="C83" s="22"/>
     </row>
-    <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="23"/>
       <c r="C84" s="22"/>
     </row>
-    <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="23"/>
       <c r="C85" s="22"/>
     </row>
-    <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="23"/>
       <c r="C86" s="22"/>
     </row>
-    <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="23"/>
       <c r="C87" s="22"/>
     </row>
-    <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="23"/>
       <c r="C88" s="22"/>
     </row>
-    <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="23"/>
       <c r="C89" s="22"/>
     </row>
-    <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="23"/>
       <c r="C90" s="22"/>
     </row>
-    <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="23"/>
       <c r="C91" s="22"/>
     </row>
-    <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="23"/>
       <c r="C92" s="22"/>
     </row>
-    <row r="93" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="23"/>
       <c r="C93" s="22"/>
     </row>
-    <row r="94" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="23"/>
       <c r="C94" s="22"/>
     </row>
-    <row r="95" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="23"/>
       <c r="C95" s="22"/>
     </row>
-    <row r="96" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="23"/>
       <c r="C96" s="22"/>
     </row>
-    <row r="97" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="23"/>
       <c r="C97" s="22"/>
     </row>
-    <row r="98" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="23"/>
       <c r="C98" s="22"/>
     </row>
-    <row r="99" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="23"/>
       <c r="C99" s="22"/>
     </row>
-    <row r="100" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="23"/>
       <c r="C100" s="22"/>
     </row>
-    <row r="101" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="23"/>
       <c r="C101" s="22"/>
     </row>
-    <row r="102" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="23"/>
       <c r="C102" s="22"/>
     </row>
-    <row r="103" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="23"/>
       <c r="C103" s="22"/>
     </row>
-    <row r="104" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="23"/>
       <c r="C104" s="22"/>
     </row>
-    <row r="105" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="23"/>
       <c r="C105" s="22"/>
     </row>
-    <row r="106" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="23"/>
       <c r="C106" s="22"/>
     </row>
-    <row r="107" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="23"/>
       <c r="C107" s="22"/>
     </row>
-    <row r="108" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="23"/>
       <c r="C108" s="22"/>
     </row>
-    <row r="109" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="23"/>
       <c r="C109" s="22"/>
     </row>
-    <row r="110" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="23"/>
       <c r="C110" s="22"/>
     </row>
-    <row r="111" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="23"/>
       <c r="C111" s="22"/>
     </row>
-    <row r="112" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="23"/>
       <c r="C112" s="22"/>
     </row>
-    <row r="113" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="23"/>
       <c r="C113" s="22"/>
     </row>
-    <row r="114" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="23"/>
       <c r="C114" s="22"/>
     </row>
-    <row r="115" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="23"/>
       <c r="C115" s="22"/>
     </row>
-    <row r="116" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="23"/>
       <c r="C116" s="22"/>
     </row>
-    <row r="117" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="23"/>
       <c r="C117" s="22"/>
     </row>
-    <row r="118" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="23"/>
       <c r="C118" s="22"/>
     </row>
-    <row r="119" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="23"/>
       <c r="C119" s="22"/>
     </row>
-    <row r="120" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="23"/>
       <c r="C120" s="22"/>
     </row>
-    <row r="121" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="23"/>
       <c r="C121" s="22"/>
     </row>
-    <row r="122" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="23"/>
       <c r="C122" s="22"/>
     </row>
-    <row r="123" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="23"/>
       <c r="C123" s="22"/>
     </row>
-    <row r="124" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="23"/>
       <c r="C124" s="22"/>
     </row>
-    <row r="125" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="23"/>
       <c r="C125" s="22"/>
     </row>
-    <row r="126" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="23"/>
       <c r="C126" s="22"/>
     </row>
-    <row r="127" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="23"/>
       <c r="C127" s="22"/>
     </row>
-    <row r="128" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="23"/>
       <c r="C128" s="22"/>
     </row>
-    <row r="129" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="23"/>
       <c r="C129" s="22"/>
     </row>
-    <row r="130" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="23"/>
       <c r="C130" s="22"/>
     </row>
-    <row r="131" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="23"/>
       <c r="C131" s="22"/>
     </row>
-    <row r="132" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="23"/>
       <c r="C132" s="22"/>
     </row>
-    <row r="133" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="23"/>
       <c r="C133" s="22"/>
     </row>
-    <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="23"/>
       <c r="C134" s="22"/>
     </row>
-    <row r="135" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="23"/>
       <c r="C135" s="22"/>
     </row>
-    <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="23"/>
       <c r="C136" s="22"/>
     </row>
-    <row r="137" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="23"/>
       <c r="C137" s="22"/>
     </row>
-    <row r="138" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="23"/>
       <c r="C138" s="22"/>
     </row>
-    <row r="139" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="23"/>
       <c r="C139" s="22"/>
     </row>
-    <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="23"/>
       <c r="C140" s="22"/>
     </row>
-    <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="23"/>
       <c r="C141" s="22"/>
     </row>
-    <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="23"/>
       <c r="C142" s="22"/>
     </row>
-    <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="23"/>
       <c r="C143" s="22"/>
     </row>
-    <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="23"/>
       <c r="C144" s="22"/>
     </row>
-    <row r="145" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="23"/>
       <c r="C145" s="22"/>
     </row>
-    <row r="146" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="23"/>
       <c r="C146" s="22"/>
     </row>
-    <row r="147" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="23"/>
       <c r="C147" s="22"/>
     </row>
-    <row r="148" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="23"/>
       <c r="C148" s="22"/>
     </row>
-    <row r="149" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="23"/>
       <c r="C149" s="22"/>
     </row>
-    <row r="150" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="23"/>
       <c r="C150" s="22"/>
     </row>
-    <row r="151" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="23"/>
       <c r="C151" s="22"/>
     </row>
-    <row r="152" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="23"/>
       <c r="C152" s="22"/>
     </row>
-    <row r="153" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="23"/>
       <c r="C153" s="22"/>
     </row>
-    <row r="154" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="23"/>
       <c r="C154" s="22"/>
     </row>
-    <row r="155" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="23"/>
       <c r="C155" s="22"/>
     </row>
-    <row r="156" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="23"/>
       <c r="C156" s="22"/>
     </row>
-    <row r="157" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="23"/>
       <c r="C157" s="22"/>
     </row>
-    <row r="158" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="23"/>
       <c r="C158" s="22"/>
     </row>
-    <row r="159" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="23"/>
       <c r="C159" s="22"/>
     </row>
-    <row r="160" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="23"/>
       <c r="C160" s="22"/>
     </row>
-    <row r="161" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="23"/>
       <c r="C161" s="22"/>
     </row>
-    <row r="162" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="23"/>
       <c r="C162" s="22"/>
     </row>
-    <row r="163" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="23"/>
       <c r="C163" s="22"/>
     </row>
-    <row r="164" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="23"/>
       <c r="C164" s="22"/>
     </row>
-    <row r="165" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="23"/>
       <c r="C165" s="22"/>
     </row>
-    <row r="166" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="23"/>
       <c r="C166" s="22"/>
     </row>
-    <row r="167" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="23"/>
       <c r="C167" s="22"/>
     </row>
-    <row r="168" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="23"/>
       <c r="C168" s="22"/>
     </row>
-    <row r="169" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="23"/>
       <c r="C169" s="22"/>
     </row>
-    <row r="170" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="23"/>
       <c r="C170" s="22"/>
     </row>
-    <row r="171" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="23"/>
       <c r="C171" s="22"/>
     </row>
-    <row r="172" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="23"/>
       <c r="C172" s="22"/>
     </row>
-    <row r="173" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="23"/>
       <c r="C173" s="22"/>
     </row>
-    <row r="174" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="23"/>
       <c r="C174" s="22"/>
     </row>
-    <row r="175" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="23"/>
       <c r="C175" s="22"/>
     </row>
-    <row r="176" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="23"/>
       <c r="C176" s="22"/>
     </row>
-    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="23"/>
       <c r="C177" s="22"/>
     </row>
-    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="23"/>
       <c r="C178" s="22"/>
     </row>
-    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="23"/>
       <c r="C179" s="22"/>
     </row>
-    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="23"/>
       <c r="C180" s="22"/>
     </row>
-    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="23"/>
       <c r="C181" s="22"/>
     </row>
-    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="23"/>
       <c r="C182" s="22"/>
     </row>
-    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="23"/>
       <c r="C183" s="22"/>
     </row>
-    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="23"/>
       <c r="C184" s="22"/>
     </row>
-    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="23"/>
       <c r="C185" s="22"/>
     </row>
-    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="23"/>
       <c r="C186" s="22"/>
     </row>
-    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="23"/>
       <c r="C187" s="22"/>
     </row>
-    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="23"/>
       <c r="C188" s="22"/>
     </row>
-    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="23"/>
       <c r="C189" s="22"/>
     </row>
-    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="23"/>
       <c r="C190" s="22"/>
     </row>
-    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="23"/>
       <c r="C191" s="22"/>
     </row>
-    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="23"/>
       <c r="C192" s="22"/>
     </row>
-    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="23"/>
       <c r="C193" s="22"/>
     </row>
-    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="23"/>
       <c r="C194" s="22"/>
     </row>
-    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="23"/>
       <c r="C195" s="22"/>
     </row>
-    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="23"/>
       <c r="C196" s="22"/>
     </row>
-    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="23"/>
       <c r="C197" s="22"/>
     </row>
-    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="23"/>
       <c r="C198" s="22"/>
     </row>
-    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="23"/>
       <c r="C199" s="22"/>
     </row>
-    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="23"/>
       <c r="C200" s="22"/>
     </row>
-    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="23"/>
       <c r="C201" s="22"/>
     </row>
-    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="23"/>
       <c r="C202" s="22"/>
     </row>
-    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="23"/>
       <c r="C203" s="22"/>
     </row>
-    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="23"/>
       <c r="C204" s="22"/>
     </row>
-    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="23"/>
       <c r="C205" s="22"/>
     </row>
-    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="23"/>
       <c r="C206" s="22"/>
     </row>
-    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="23"/>
       <c r="C207" s="22"/>
     </row>
-    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="23"/>
       <c r="C208" s="22"/>
     </row>
-    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="23"/>
       <c r="C209" s="22"/>
     </row>
-    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="23"/>
       <c r="C210" s="22"/>
     </row>
-    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="23"/>
       <c r="C211" s="22"/>
     </row>
-    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="23"/>
       <c r="C212" s="22"/>
     </row>
-    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="23"/>
       <c r="C213" s="22"/>
     </row>
-    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="23"/>
       <c r="C214" s="22"/>
     </row>
-    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="23"/>
       <c r="C215" s="22"/>
     </row>
-    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="23"/>
       <c r="C216" s="22"/>
     </row>
-    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="23"/>
       <c r="C217" s="22"/>
     </row>
-    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="23"/>
       <c r="C218" s="22"/>
     </row>
-    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="23"/>
       <c r="C219" s="22"/>
     </row>
-    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="23"/>
       <c r="C220" s="22"/>
     </row>
-    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="23"/>
       <c r="C221" s="22"/>
     </row>
-    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="23"/>
       <c r="C222" s="22"/>
     </row>
-    <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="23"/>
       <c r="C223" s="22"/>
     </row>
-    <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="23"/>
       <c r="C224" s="22"/>
     </row>
-    <row r="225" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="23"/>
       <c r="C225" s="22"/>
     </row>
-    <row r="226" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="23"/>
       <c r="C226" s="22"/>
     </row>
-    <row r="227" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="23"/>
       <c r="C227" s="22"/>
     </row>
-    <row r="228" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="23"/>
       <c r="C228" s="22"/>
     </row>
-    <row r="229" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="23"/>
       <c r="C229" s="22"/>
     </row>
-    <row r="230" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="23"/>
       <c r="C230" s="22"/>
     </row>
-    <row r="231" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="23"/>
       <c r="C231" s="22"/>
     </row>
-    <row r="232" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="23"/>
       <c r="C232" s="22"/>
     </row>
-    <row r="233" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="23"/>
       <c r="C233" s="22"/>
     </row>
-    <row r="234" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="23"/>
       <c r="C234" s="22"/>
     </row>
-    <row r="235" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="23"/>
       <c r="C235" s="22"/>
     </row>
-    <row r="236" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="23"/>
       <c r="C236" s="22"/>
     </row>
-    <row r="237" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="23"/>
       <c r="C237" s="22"/>
     </row>
-    <row r="238" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="23"/>
       <c r="C238" s="22"/>
     </row>
-    <row r="239" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="23"/>
       <c r="C239" s="22"/>
     </row>
-    <row r="240" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="23"/>
       <c r="C240" s="22"/>
     </row>
-    <row r="241" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="23"/>
       <c r="C241" s="22"/>
     </row>
-    <row r="242" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="23"/>
       <c r="C242" s="22"/>
     </row>
-    <row r="243" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="23"/>
       <c r="C243" s="22"/>
     </row>
-    <row r="244" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="23"/>
       <c r="C244" s="22"/>
     </row>
-    <row r="245" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="23"/>
       <c r="C245" s="22"/>
     </row>
-    <row r="246" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="23"/>
       <c r="C246" s="22"/>
     </row>
-    <row r="247" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="23"/>
       <c r="C247" s="22"/>
     </row>
-    <row r="248" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="23"/>
       <c r="C248" s="22"/>
     </row>
-    <row r="249" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="23"/>
       <c r="C249" s="22"/>
     </row>
-    <row r="250" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="23"/>
       <c r="C250" s="22"/>
     </row>
-    <row r="251" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="23"/>
       <c r="C251" s="22"/>
     </row>
-    <row r="252" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="23"/>
       <c r="C252" s="22"/>
     </row>
-    <row r="253" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="23"/>
       <c r="C253" s="22"/>
     </row>
-    <row r="254" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="23"/>
       <c r="C254" s="22"/>
     </row>
-    <row r="255" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="23"/>
       <c r="C255" s="22"/>
     </row>
-    <row r="256" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="23"/>
       <c r="C256" s="22"/>
     </row>
-    <row r="257" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="23"/>
       <c r="C257" s="22"/>
     </row>
-    <row r="258" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="23"/>
       <c r="C258" s="22"/>
     </row>
-    <row r="259" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="23"/>
       <c r="C259" s="22"/>
     </row>
-    <row r="260" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A260" s="23"/>
       <c r="C260" s="22"/>
     </row>
-    <row r="261" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="23"/>
       <c r="C261" s="22"/>
     </row>
-    <row r="262" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="23"/>
       <c r="C262" s="22"/>
     </row>
-    <row r="263" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="23"/>
       <c r="C263" s="22"/>
     </row>
-    <row r="264" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="23"/>
       <c r="C264" s="22"/>
     </row>
-    <row r="265" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" s="23"/>
       <c r="C265" s="22"/>
     </row>
-    <row r="266" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A266" s="23"/>
       <c r="C266" s="22"/>
     </row>
-    <row r="267" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A267" s="23"/>
       <c r="C267" s="22"/>
     </row>
-    <row r="268" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268" s="23"/>
       <c r="C268" s="22"/>
     </row>
-    <row r="269" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" s="23"/>
       <c r="C269" s="22"/>
     </row>
-    <row r="270" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="23"/>
       <c r="C270" s="22"/>
     </row>
-    <row r="271" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A271" s="23"/>
       <c r="C271" s="22"/>
     </row>
-    <row r="272" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A272" s="23"/>
       <c r="C272" s="22"/>
     </row>
-    <row r="273" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A273" s="23"/>
       <c r="C273" s="22"/>
     </row>
-    <row r="274" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A274" s="23"/>
       <c r="C274" s="22"/>
     </row>
-    <row r="275" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A275" s="23"/>
       <c r="C275" s="22"/>
     </row>
-    <row r="276" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A276" s="23"/>
       <c r="C276" s="22"/>
     </row>
-    <row r="277" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A277" s="23"/>
       <c r="C277" s="22"/>
     </row>
-    <row r="278" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A278" s="23"/>
       <c r="C278" s="22"/>
     </row>
-    <row r="279" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A279" s="23"/>
       <c r="C279" s="22"/>
     </row>
-    <row r="280" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C280" s="22"/>
     </row>
-    <row r="281" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C281" s="22"/>
     </row>
-    <row r="282" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C282" s="22"/>
     </row>
-    <row r="283" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C283" s="22"/>
     </row>
-    <row r="284" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C284" s="22"/>
     </row>
-    <row r="285" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C285" s="22"/>
     </row>
-    <row r="286" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C286" s="22"/>
     </row>
-    <row r="287" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C287" s="22"/>
     </row>
-    <row r="288" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C288" s="22"/>
     </row>
-    <row r="289" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C289" s="22"/>
     </row>
-    <row r="290" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C290" s="22"/>
     </row>
-    <row r="291" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C291" s="22"/>
     </row>
-    <row r="292" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C292" s="22"/>
     </row>
-    <row r="293" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C293" s="22"/>
     </row>
-    <row r="294" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C294" s="22"/>
     </row>
-    <row r="295" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C295" s="22"/>
     </row>
-    <row r="296" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C296" s="22"/>
     </row>
-    <row r="297" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C297" s="22"/>
     </row>
-    <row r="298" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C298" s="22"/>
     </row>
-    <row r="299" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C299" s="22"/>
     </row>
-    <row r="300" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C300" s="22"/>
     </row>
-    <row r="301" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C301" s="22"/>
     </row>
-    <row r="302" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C302" s="22"/>
     </row>
-    <row r="303" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C303" s="22"/>
     </row>
-    <row r="304" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C304" s="22"/>
     </row>
-    <row r="305" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C305" s="22"/>
     </row>
-    <row r="306" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C306" s="22"/>
     </row>
-    <row r="307" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C307" s="22"/>
     </row>
-    <row r="308" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C308" s="22"/>
     </row>
-    <row r="309" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C309" s="22"/>
     </row>
-    <row r="310" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C310" s="22"/>
     </row>
-    <row r="311" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C311" s="22"/>
     </row>
-    <row r="312" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C312" s="22"/>
     </row>
-    <row r="313" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C313" s="22"/>
     </row>
-    <row r="314" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C314" s="22"/>
     </row>
-    <row r="315" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C315" s="22"/>
     </row>
-    <row r="316" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C316" s="22"/>
     </row>
-    <row r="317" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C317" s="22"/>
     </row>
-    <row r="318" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C318" s="22"/>
     </row>
-    <row r="319" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C319" s="22"/>
     </row>
-    <row r="320" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C320" s="22"/>
     </row>
-    <row r="321" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C321" s="22"/>
     </row>
-    <row r="322" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C322" s="22"/>
     </row>
-    <row r="323" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C323" s="22"/>
     </row>
-    <row r="324" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C324" s="22"/>
     </row>
-    <row r="325" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C325" s="22"/>
     </row>
-    <row r="326" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C326" s="22"/>
     </row>
-    <row r="327" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C327" s="22"/>
     </row>
-    <row r="328" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C328" s="22"/>
     </row>
-    <row r="329" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C329" s="22"/>
     </row>
-    <row r="330" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C330" s="22"/>
     </row>
-    <row r="331" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C331" s="22"/>
     </row>
-    <row r="332" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C332" s="22"/>
     </row>
-    <row r="333" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C333" s="22"/>
     </row>
-    <row r="334" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C334" s="22"/>
     </row>
-    <row r="335" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="335" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C335" s="22"/>
     </row>
-    <row r="336" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C336" s="22"/>
     </row>
-    <row r="337" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="337" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C337" s="22"/>
     </row>
-    <row r="338" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C338" s="22"/>
     </row>
-    <row r="339" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C339" s="22"/>
     </row>
-    <row r="340" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C340" s="22"/>
     </row>
-    <row r="341" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C341" s="22"/>
     </row>
-    <row r="342" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="342" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C342" s="22"/>
     </row>
-    <row r="343" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="343" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C343" s="22"/>
     </row>
-    <row r="344" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="344" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C344" s="22"/>
     </row>
-    <row r="345" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="345" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C345" s="22"/>
     </row>
-    <row r="346" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="346" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C346" s="22"/>
     </row>
-    <row r="347" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="347" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C347" s="22"/>
     </row>
-    <row r="348" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="348" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C348" s="22"/>
     </row>
-    <row r="349" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="349" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C349" s="22"/>
     </row>
-    <row r="350" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="350" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C350" s="22"/>
     </row>
-    <row r="351" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="351" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C351" s="22"/>
     </row>
-    <row r="352" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="352" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C352" s="22"/>
     </row>
-    <row r="353" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="353" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C353" s="22"/>
     </row>
-    <row r="354" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="354" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C354" s="22"/>
     </row>
-    <row r="355" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="355" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C355" s="22"/>
     </row>
-    <row r="356" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="356" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C356" s="22"/>
     </row>
-    <row r="357" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="357" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C357" s="22"/>
     </row>
-    <row r="358" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="358" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C358" s="22"/>
     </row>
-    <row r="359" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="359" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C359" s="22"/>
     </row>
-    <row r="360" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="360" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C360" s="22"/>
     </row>
-    <row r="361" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="361" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C361" s="22"/>
     </row>
-    <row r="362" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="362" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C362" s="22"/>
     </row>
-    <row r="363" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="363" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C363" s="22"/>
     </row>
-    <row r="364" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="364" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C364" s="22"/>
     </row>
-    <row r="365" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="365" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C365" s="22"/>
     </row>
-    <row r="366" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="366" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C366" s="22"/>
     </row>
-    <row r="367" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="367" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C367" s="22"/>
     </row>
-    <row r="368" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="368" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C368" s="22"/>
     </row>
-    <row r="369" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="369" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C369" s="22"/>
     </row>
-    <row r="370" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="370" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C370" s="22"/>
     </row>
-    <row r="371" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="371" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C371" s="22"/>
     </row>
-    <row r="372" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="372" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C372" s="22"/>
     </row>
-    <row r="373" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="373" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C373" s="22"/>
     </row>
-    <row r="374" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="374" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C374" s="22"/>
     </row>
-    <row r="375" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="375" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C375" s="22"/>
     </row>
-    <row r="376" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="376" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C376" s="22"/>
     </row>
-    <row r="377" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="377" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C377" s="22"/>
     </row>
-    <row r="378" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="378" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C378" s="22"/>
     </row>
-    <row r="379" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="379" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C379" s="22"/>
     </row>
-    <row r="380" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="380" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C380" s="22"/>
     </row>
-    <row r="381" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="381" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C381" s="22"/>
     </row>
-    <row r="382" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="382" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C382" s="22"/>
     </row>
-    <row r="383" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="383" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C383" s="22"/>
     </row>
-    <row r="384" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="384" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C384" s="22"/>
     </row>
-    <row r="385" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="385" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C385" s="22"/>
     </row>
-    <row r="386" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="386" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C386" s="22"/>
     </row>
-    <row r="387" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="387" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C387" s="22"/>
     </row>
-    <row r="388" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="388" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C388" s="22"/>
     </row>
-    <row r="389" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="389" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C389" s="22"/>
     </row>
-    <row r="390" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="390" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C390" s="22"/>
     </row>
-    <row r="391" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="391" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C391" s="22"/>
     </row>
-    <row r="392" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="392" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C392" s="22"/>
     </row>
-    <row r="393" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="393" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C393" s="22"/>
     </row>
-    <row r="394" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="394" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C394" s="22"/>
     </row>
-    <row r="395" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="395" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C395" s="22"/>
     </row>
-    <row r="396" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="396" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C396" s="22"/>
     </row>
-    <row r="397" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="397" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C397" s="22"/>
     </row>
-    <row r="398" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="398" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C398" s="22"/>
     </row>
-    <row r="399" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="399" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C399" s="22"/>
     </row>
-    <row r="400" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="400" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C400" s="22"/>
     </row>
-    <row r="401" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="401" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C401" s="22"/>
     </row>
-    <row r="402" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="402" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C402" s="22"/>
     </row>
-    <row r="403" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="403" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C403" s="22"/>
     </row>
-    <row r="404" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="404" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C404" s="22"/>
     </row>
-    <row r="405" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="405" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C405" s="22"/>
     </row>
-    <row r="406" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="406" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C406" s="22"/>
     </row>
-    <row r="407" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="407" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C407" s="22"/>
     </row>
-    <row r="408" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="408" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C408" s="22"/>
     </row>
-    <row r="409" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="409" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C409" s="22"/>
     </row>
-    <row r="410" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="410" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C410" s="22"/>
     </row>
-    <row r="411" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="411" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C411" s="22"/>
     </row>
-    <row r="412" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="412" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C412" s="22"/>
     </row>
-    <row r="413" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="413" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C413" s="22"/>
     </row>
-    <row r="414" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="414" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C414" s="22"/>
     </row>
-    <row r="415" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="415" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C415" s="22"/>
     </row>
-    <row r="416" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="416" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C416" s="22"/>
     </row>
-    <row r="417" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="417" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C417" s="22"/>
     </row>
-    <row r="418" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="418" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C418" s="22"/>
     </row>
-    <row r="419" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="419" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C419" s="22"/>
     </row>
-    <row r="420" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="420" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C420" s="22"/>
     </row>
-    <row r="421" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="421" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C421" s="22"/>
     </row>
-    <row r="422" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="422" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C422" s="22"/>
     </row>
-    <row r="423" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="423" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C423" s="22"/>
     </row>
-    <row r="424" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="424" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C424" s="22"/>
     </row>
-    <row r="425" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="425" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C425" s="22"/>
     </row>
-    <row r="426" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="426" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C426" s="22"/>
     </row>
-    <row r="427" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="427" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C427" s="22"/>
     </row>
-    <row r="428" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="428" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C428" s="22"/>
     </row>
-    <row r="429" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="429" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C429" s="22"/>
     </row>
-    <row r="430" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="430" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C430" s="22"/>
     </row>
-    <row r="431" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="431" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C431" s="22"/>
     </row>
-    <row r="432" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="432" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C432" s="22"/>
     </row>
-    <row r="433" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="433" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C433" s="22"/>
     </row>
-    <row r="434" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="434" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C434" s="22"/>
     </row>
-    <row r="435" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="435" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C435" s="22"/>
     </row>
-    <row r="436" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="436" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C436" s="22"/>
     </row>
-    <row r="437" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="437" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C437" s="22"/>
     </row>
-    <row r="438" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="438" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C438" s="22"/>
     </row>
-    <row r="439" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="439" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C439" s="22"/>
     </row>
-    <row r="440" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="440" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C440" s="22"/>
     </row>
-    <row r="441" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="441" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C441" s="22"/>
     </row>
-    <row r="442" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="442" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C442" s="22"/>
     </row>
-    <row r="443" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="443" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C443" s="22"/>
     </row>
-    <row r="444" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="444" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C444" s="22"/>
     </row>
-    <row r="445" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="445" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C445" s="22"/>
     </row>
-    <row r="446" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="446" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C446" s="22"/>
     </row>
-    <row r="447" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="447" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C447" s="22"/>
     </row>
-    <row r="448" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="448" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C448" s="22"/>
     </row>
-    <row r="449" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="449" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C449" s="22"/>
     </row>
-    <row r="450" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="450" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C450" s="22"/>
     </row>
-    <row r="451" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="451" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C451" s="22"/>
     </row>
-    <row r="452" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="452" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C452" s="22"/>
     </row>
-    <row r="453" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="453" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C453" s="22"/>
     </row>
-    <row r="454" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="454" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C454" s="22"/>
     </row>
-    <row r="455" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="455" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C455" s="22"/>
     </row>
-    <row r="456" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="456" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C456" s="22"/>
     </row>
-    <row r="457" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="457" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C457" s="22"/>
     </row>
-    <row r="458" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="458" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C458" s="22"/>
     </row>
-    <row r="459" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="459" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C459" s="22"/>
     </row>
-    <row r="460" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="460" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C460" s="22"/>
     </row>
-    <row r="461" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="461" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C461" s="22"/>
     </row>
-    <row r="462" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="462" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C462" s="22"/>
     </row>
-    <row r="463" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="463" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C463" s="22"/>
     </row>
-    <row r="464" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="464" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C464" s="22"/>
     </row>
-    <row r="465" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="465" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C465" s="22"/>
     </row>
-    <row r="466" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="466" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C466" s="22"/>
     </row>
-    <row r="467" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="467" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C467" s="22"/>
     </row>
-    <row r="468" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="468" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C468" s="22"/>
     </row>
-    <row r="469" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="469" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C469" s="22"/>
     </row>
-    <row r="470" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="470" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C470" s="22"/>
     </row>
-    <row r="471" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="471" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C471" s="22"/>
     </row>
-    <row r="472" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="472" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C472" s="22"/>
     </row>
-    <row r="473" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="473" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C473" s="22"/>
     </row>
-    <row r="474" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="474" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C474" s="22"/>
     </row>
-    <row r="475" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="475" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C475" s="22"/>
     </row>
-    <row r="476" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="476" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C476" s="22"/>
     </row>
-    <row r="477" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="477" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C477" s="22"/>
     </row>
-    <row r="478" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="478" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C478" s="22"/>
     </row>
-    <row r="479" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="479" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C479" s="22"/>
     </row>
-    <row r="480" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="480" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C480" s="22"/>
     </row>
-    <row r="481" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="481" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C481" s="22"/>
     </row>
-    <row r="482" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="482" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C482" s="22"/>
     </row>
-    <row r="483" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="483" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C483" s="22"/>
     </row>
-    <row r="484" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="484" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C484" s="22"/>
     </row>
-    <row r="485" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="485" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C485" s="22"/>
     </row>
-    <row r="486" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="486" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C486" s="22"/>
     </row>
-    <row r="487" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="487" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C487" s="22"/>
     </row>
-    <row r="488" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="488" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C488" s="22"/>
     </row>
-    <row r="489" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="489" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C489" s="22"/>
     </row>
-    <row r="490" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="490" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C490" s="22"/>
     </row>
-    <row r="491" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="491" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C491" s="22"/>
     </row>
-    <row r="492" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="492" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C492" s="22"/>
     </row>
-    <row r="493" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="493" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C493" s="22"/>
     </row>
-    <row r="494" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="494" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C494" s="22"/>
     </row>
-    <row r="495" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="495" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C495" s="22"/>
     </row>
-    <row r="496" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="496" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C496" s="22"/>
     </row>
-    <row r="497" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="497" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C497" s="22"/>
     </row>
-    <row r="498" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="498" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C498" s="22"/>
     </row>
-    <row r="499" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="499" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C499" s="22"/>
     </row>
-    <row r="500" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="500" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C500" s="22"/>
     </row>
-    <row r="501" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="501" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C501" s="22"/>
     </row>
-    <row r="502" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="502" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C502" s="22"/>
     </row>
-    <row r="503" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="503" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C503" s="22"/>
     </row>
-    <row r="504" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="504" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C504" s="22"/>
     </row>
-    <row r="505" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="505" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C505" s="22"/>
     </row>
-    <row r="506" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="506" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C506" s="22"/>
     </row>
-    <row r="507" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="507" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C507" s="22"/>
     </row>
-    <row r="508" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="508" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C508" s="22"/>
     </row>
-    <row r="509" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="509" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C509" s="22"/>
     </row>
-    <row r="510" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="510" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C510" s="22"/>
     </row>
-    <row r="511" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="511" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C511" s="22"/>
     </row>
-    <row r="512" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="512" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C512" s="22"/>
     </row>
-    <row r="513" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="513" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C513" s="22"/>
     </row>
-    <row r="514" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="514" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C514" s="22"/>
     </row>
-    <row r="515" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="515" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C515" s="22"/>
     </row>
-    <row r="516" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="516" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C516" s="22"/>
     </row>
-    <row r="517" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="517" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C517" s="22"/>
     </row>
-    <row r="518" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="518" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C518" s="22"/>
     </row>
-    <row r="519" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="519" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C519" s="22"/>
     </row>
-    <row r="520" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="520" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C520" s="22"/>
     </row>
-    <row r="521" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="521" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C521" s="22"/>
     </row>
-    <row r="522" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="522" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C522" s="22"/>
     </row>
-    <row r="523" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="523" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C523" s="22"/>
     </row>
-    <row r="524" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="524" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C524" s="22"/>
     </row>
-    <row r="525" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="525" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C525" s="22"/>
     </row>
-    <row r="526" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="526" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C526" s="22"/>
     </row>
-    <row r="527" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="527" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C527" s="22"/>
     </row>
-    <row r="528" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="528" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C528" s="22"/>
     </row>
-    <row r="529" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="529" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C529" s="22"/>
     </row>
-    <row r="530" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="530" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C530" s="22"/>
     </row>
-    <row r="531" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="531" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C531" s="22"/>
     </row>
-    <row r="532" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="532" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C532" s="22"/>
     </row>
-    <row r="533" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="533" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C533" s="22"/>
     </row>
-    <row r="534" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="534" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C534" s="22"/>
     </row>
-    <row r="535" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="535" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C535" s="22"/>
     </row>
-    <row r="536" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="536" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C536" s="22"/>
     </row>
-    <row r="537" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="537" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C537" s="22"/>
     </row>
-    <row r="538" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="538" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C538" s="22"/>
     </row>
-    <row r="539" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="539" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C539" s="22"/>
     </row>
-    <row r="540" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="540" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C540" s="22"/>
     </row>
-    <row r="541" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="541" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C541" s="22"/>
     </row>
-    <row r="542" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="542" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C542" s="22"/>
     </row>
-    <row r="543" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="543" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C543" s="22"/>
     </row>
-    <row r="544" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="544" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C544" s="22"/>
     </row>
-    <row r="545" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="545" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C545" s="22"/>
     </row>
-    <row r="546" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="546" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C546" s="22"/>
     </row>
-    <row r="547" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="547" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C547" s="22"/>
     </row>
-    <row r="548" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="548" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C548" s="22"/>
     </row>
-    <row r="549" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="549" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C549" s="22"/>
     </row>
-    <row r="550" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="550" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C550" s="22"/>
     </row>
-    <row r="551" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="551" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C551" s="22"/>
     </row>
-    <row r="552" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="552" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C552" s="22"/>
     </row>
-    <row r="553" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="553" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C553" s="22"/>
     </row>
-    <row r="554" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="554" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C554" s="22"/>
     </row>
-    <row r="555" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="555" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C555" s="22"/>
     </row>
-    <row r="556" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="556" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C556" s="22"/>
     </row>
-    <row r="557" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="557" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C557" s="22"/>
     </row>
-    <row r="558" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="558" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C558" s="22"/>
     </row>
-    <row r="559" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="559" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C559" s="22"/>
     </row>
-    <row r="560" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="560" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C560" s="22"/>
     </row>
-    <row r="561" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="561" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C561" s="22"/>
     </row>
-    <row r="562" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="562" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C562" s="22"/>
     </row>
-    <row r="563" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="563" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C563" s="22"/>
     </row>
-    <row r="564" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="564" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C564" s="22"/>
     </row>
-    <row r="565" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="565" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C565" s="22"/>
     </row>
-    <row r="566" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="566" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C566" s="22"/>
     </row>
-    <row r="567" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="567" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C567" s="22"/>
     </row>
-    <row r="568" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="568" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C568" s="22"/>
     </row>
-    <row r="569" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="569" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C569" s="22"/>
     </row>
-    <row r="570" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="570" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C570" s="22"/>
     </row>
-    <row r="571" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="571" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C571" s="22"/>
     </row>
-    <row r="572" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="572" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C572" s="22"/>
     </row>
-    <row r="573" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="573" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C573" s="22"/>
     </row>
-    <row r="574" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="574" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C574" s="22"/>
     </row>
-    <row r="575" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="575" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C575" s="22"/>
     </row>
-    <row r="576" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="576" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C576" s="22"/>
     </row>
-    <row r="577" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="577" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C577" s="22"/>
     </row>
-    <row r="578" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="578" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C578" s="22"/>
     </row>
-    <row r="579" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="579" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C579" s="22"/>
     </row>
-    <row r="580" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="580" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C580" s="22"/>
     </row>
-    <row r="581" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="581" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C581" s="22"/>
     </row>
-    <row r="582" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="582" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C582" s="22"/>
     </row>
-    <row r="583" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="583" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C583" s="22"/>
     </row>
-    <row r="584" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="584" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C584" s="22"/>
     </row>
-    <row r="585" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="585" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C585" s="22"/>
     </row>
-    <row r="586" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="586" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C586" s="22"/>
     </row>
-    <row r="587" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="587" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C587" s="22"/>
     </row>
-    <row r="588" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="588" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C588" s="22"/>
     </row>
-    <row r="589" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="589" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C589" s="22"/>
     </row>
-    <row r="590" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="590" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C590" s="22"/>
     </row>
-    <row r="591" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="591" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C591" s="22"/>
     </row>
-    <row r="592" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="592" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C592" s="22"/>
     </row>
-    <row r="593" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="593" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C593" s="22"/>
     </row>
-    <row r="594" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="594" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C594" s="22"/>
     </row>
-    <row r="595" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="595" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C595" s="22"/>
     </row>
-    <row r="596" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="596" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C596" s="22"/>
     </row>
-    <row r="597" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="597" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C597" s="22"/>
     </row>
-    <row r="598" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="598" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C598" s="22"/>
     </row>
-    <row r="599" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="599" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C599" s="22"/>
     </row>
-    <row r="600" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="600" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C600" s="22"/>
     </row>
-    <row r="601" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="601" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C601" s="22"/>
     </row>
-    <row r="602" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="602" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C602" s="22"/>
     </row>
-    <row r="603" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="603" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C603" s="22"/>
     </row>
-    <row r="604" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="604" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C604" s="22"/>
     </row>
-    <row r="605" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="605" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C605" s="22"/>
     </row>
-    <row r="606" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="606" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C606" s="22"/>
     </row>
-    <row r="607" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="607" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C607" s="22"/>
     </row>
-    <row r="608" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="608" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C608" s="22"/>
     </row>
-    <row r="609" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="609" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C609" s="22"/>
     </row>
-    <row r="610" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="610" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C610" s="22"/>
     </row>
-    <row r="611" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="611" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C611" s="22"/>
     </row>
-    <row r="612" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="612" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C612" s="22"/>
     </row>
-    <row r="613" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="613" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C613" s="22"/>
     </row>
-    <row r="614" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="614" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C614" s="22"/>
     </row>
-    <row r="615" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="615" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C615" s="22"/>
     </row>
-    <row r="616" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="616" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C616" s="22"/>
     </row>
-    <row r="617" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="617" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C617" s="22"/>
     </row>
-    <row r="618" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="618" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C618" s="22"/>
     </row>
-    <row r="619" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="619" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C619" s="22"/>
     </row>
-    <row r="620" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="620" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C620" s="22"/>
     </row>
-    <row r="621" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="621" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C621" s="22"/>
     </row>
-    <row r="622" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="622" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C622" s="22"/>
     </row>
-    <row r="623" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="623" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C623" s="22"/>
     </row>
-    <row r="624" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="624" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C624" s="22"/>
     </row>
-    <row r="625" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="625" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C625" s="22"/>
     </row>
-    <row r="626" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="626" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C626" s="22"/>
     </row>
-    <row r="627" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="627" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C627" s="22"/>
     </row>
-    <row r="628" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="628" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C628" s="22"/>
     </row>
-    <row r="629" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="629" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C629" s="22"/>
     </row>
-    <row r="630" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="630" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C630" s="22"/>
     </row>
-    <row r="631" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="631" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C631" s="22"/>
     </row>
-    <row r="632" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="632" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C632" s="22"/>
     </row>
-    <row r="633" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="633" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C633" s="22"/>
     </row>
-    <row r="634" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="634" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C634" s="22"/>
     </row>
-    <row r="635" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="635" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C635" s="22"/>
     </row>
-    <row r="636" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="636" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C636" s="22"/>
     </row>
-    <row r="637" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="637" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C637" s="22"/>
     </row>
-    <row r="638" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="638" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C638" s="22"/>
     </row>
-    <row r="639" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="639" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C639" s="22"/>
     </row>
-    <row r="640" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="640" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C640" s="22"/>
     </row>
-    <row r="641" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="641" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C641" s="22"/>
     </row>
-    <row r="642" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="642" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C642" s="22"/>
     </row>
-    <row r="643" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="643" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C643" s="22"/>
     </row>
-    <row r="644" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="644" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C644" s="22"/>
     </row>
-    <row r="645" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="645" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C645" s="22"/>
     </row>
-    <row r="646" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="646" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C646" s="22"/>
     </row>
-    <row r="647" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="647" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C647" s="22"/>
     </row>
-    <row r="648" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="648" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C648" s="22"/>
     </row>
-    <row r="649" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="649" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C649" s="22"/>
     </row>
-    <row r="650" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="650" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C650" s="22"/>
     </row>
-    <row r="651" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="651" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C651" s="22"/>
     </row>
-    <row r="652" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="652" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C652" s="22"/>
     </row>
-    <row r="653" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="653" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C653" s="22"/>
     </row>
-    <row r="654" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="654" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C654" s="22"/>
     </row>
-    <row r="655" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="655" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C655" s="22"/>
     </row>
-    <row r="656" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="656" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C656" s="22"/>
     </row>
-    <row r="657" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="657" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C657" s="22"/>
     </row>
-    <row r="658" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="658" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C658" s="22"/>
     </row>
-    <row r="659" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="659" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C659" s="22"/>
     </row>
-    <row r="660" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="660" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C660" s="22"/>
     </row>
-    <row r="661" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="661" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C661" s="22"/>
     </row>
-    <row r="662" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="662" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C662" s="22"/>
     </row>
-    <row r="663" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="663" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C663" s="22"/>
     </row>
-    <row r="664" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="664" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C664" s="22"/>
     </row>
-    <row r="665" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="665" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C665" s="22"/>
     </row>
-    <row r="666" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="666" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C666" s="22"/>
     </row>
-    <row r="667" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="667" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C667" s="22"/>
     </row>
-    <row r="668" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="668" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C668" s="22"/>
     </row>
-    <row r="669" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="669" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C669" s="22"/>
     </row>
-    <row r="670" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="670" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C670" s="22"/>
     </row>
-    <row r="671" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="671" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C671" s="22"/>
     </row>
-    <row r="672" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="672" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C672" s="22"/>
     </row>
-    <row r="673" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="673" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C673" s="22"/>
     </row>
-    <row r="674" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="674" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C674" s="22"/>
     </row>
-    <row r="675" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="675" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C675" s="22"/>
     </row>
-    <row r="676" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="676" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C676" s="22"/>
     </row>
-    <row r="677" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="677" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C677" s="22"/>
     </row>
-    <row r="678" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="678" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C678" s="22"/>
     </row>
-    <row r="679" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="679" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C679" s="22"/>
     </row>
-    <row r="680" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="680" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C680" s="22"/>
     </row>
-    <row r="681" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="681" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C681" s="22"/>
     </row>
-    <row r="682" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="682" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C682" s="22"/>
     </row>
-    <row r="683" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="683" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C683" s="22"/>
     </row>
-    <row r="684" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="684" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C684" s="22"/>
     </row>
-    <row r="685" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="685" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C685" s="22"/>
     </row>
-    <row r="686" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="686" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C686" s="22"/>
     </row>
-    <row r="687" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="687" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C687" s="22"/>
     </row>
-    <row r="688" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="688" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C688" s="22"/>
     </row>
-    <row r="689" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="689" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C689" s="22"/>
     </row>
-    <row r="690" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="690" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C690" s="22"/>
     </row>
-    <row r="691" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="691" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C691" s="22"/>
     </row>
-    <row r="692" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="692" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C692" s="22"/>
     </row>
-    <row r="693" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="693" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C693" s="22"/>
     </row>
-    <row r="694" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="694" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C694" s="22"/>
     </row>
-    <row r="695" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="695" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C695" s="22"/>
     </row>
-    <row r="696" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="696" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C696" s="22"/>
     </row>
-    <row r="697" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="697" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C697" s="22"/>
     </row>
-    <row r="698" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="698" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C698" s="22"/>
     </row>
-    <row r="699" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="699" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C699" s="22"/>
     </row>
-    <row r="700" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="700" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C700" s="22"/>
     </row>
-    <row r="701" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="701" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C701" s="22"/>
     </row>
-    <row r="702" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="702" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C702" s="22"/>
     </row>
-    <row r="703" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="703" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C703" s="22"/>
     </row>
-    <row r="704" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="704" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C704" s="22"/>
     </row>
-    <row r="705" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="705" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C705" s="22"/>
     </row>
-    <row r="706" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="706" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C706" s="22"/>
     </row>
-    <row r="707" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="707" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C707" s="22"/>
     </row>
-    <row r="708" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="708" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C708" s="22"/>
     </row>
-    <row r="709" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="709" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C709" s="22"/>
     </row>
-    <row r="710" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="710" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C710" s="22"/>
     </row>
-    <row r="711" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="711" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C711" s="22"/>
     </row>
-    <row r="712" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="712" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C712" s="22"/>
     </row>
-    <row r="713" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="713" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C713" s="22"/>
     </row>
-    <row r="714" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="714" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C714" s="22"/>
     </row>
-    <row r="715" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="715" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C715" s="22"/>
     </row>
-    <row r="716" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="716" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C716" s="22"/>
     </row>
-    <row r="717" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="717" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C717" s="22"/>
     </row>
-    <row r="718" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="718" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C718" s="22"/>
     </row>
-    <row r="719" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="719" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C719" s="22"/>
     </row>
-    <row r="720" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="720" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C720" s="22"/>
     </row>
-    <row r="721" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="721" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C721" s="22"/>
     </row>
-    <row r="722" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="722" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C722" s="22"/>
     </row>
-    <row r="723" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="723" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C723" s="22"/>
     </row>
-    <row r="724" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="724" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C724" s="22"/>
     </row>
-    <row r="725" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="725" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C725" s="22"/>
     </row>
-    <row r="726" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="726" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C726" s="22"/>
     </row>
-    <row r="727" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="727" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C727" s="22"/>
     </row>
-    <row r="728" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="728" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C728" s="22"/>
     </row>
-    <row r="729" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="729" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C729" s="22"/>
     </row>
-    <row r="730" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="730" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C730" s="22"/>
     </row>
-    <row r="731" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="731" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C731" s="22"/>
     </row>
-    <row r="732" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="732" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C732" s="22"/>
     </row>
-    <row r="733" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="733" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C733" s="22"/>
     </row>
-    <row r="734" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="734" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C734" s="22"/>
     </row>
-    <row r="735" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="735" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C735" s="22"/>
     </row>
-    <row r="736" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="736" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C736" s="22"/>
     </row>
-    <row r="737" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="737" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C737" s="22"/>
     </row>
-    <row r="738" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="738" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C738" s="22"/>
     </row>
-    <row r="739" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="739" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C739" s="22"/>
     </row>
-    <row r="740" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="740" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C740" s="22"/>
     </row>
-    <row r="741" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="741" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C741" s="22"/>
     </row>
-    <row r="742" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="742" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C742" s="22"/>
     </row>
-    <row r="743" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="743" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C743" s="22"/>
     </row>
-    <row r="744" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="744" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C744" s="22"/>
     </row>
-    <row r="745" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="745" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C745" s="22"/>
     </row>
-    <row r="746" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="746" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C746" s="22"/>
     </row>
-    <row r="747" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="747" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C747" s="22"/>
     </row>
-    <row r="748" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="748" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C748" s="22"/>
     </row>
-    <row r="749" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="749" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C749" s="22"/>
     </row>
-    <row r="750" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="750" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C750" s="22"/>
     </row>
-    <row r="751" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="751" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C751" s="22"/>
     </row>
-    <row r="752" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="752" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C752" s="22"/>
     </row>
-    <row r="753" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="753" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C753" s="22"/>
     </row>
-    <row r="754" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="754" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C754" s="22"/>
     </row>
-    <row r="755" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="755" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C755" s="22"/>
     </row>
-    <row r="756" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="756" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C756" s="22"/>
     </row>
-    <row r="757" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="757" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C757" s="22"/>
     </row>
-    <row r="758" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="758" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C758" s="22"/>
     </row>
-    <row r="759" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="759" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C759" s="22"/>
     </row>
-    <row r="760" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="760" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C760" s="22"/>
     </row>
-    <row r="761" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="761" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C761" s="22"/>
     </row>
-    <row r="762" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="762" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C762" s="22"/>
     </row>
-    <row r="763" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="763" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C763" s="22"/>
     </row>
-    <row r="764" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="764" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C764" s="22"/>
     </row>
-    <row r="765" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="765" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C765" s="22"/>
     </row>
-    <row r="766" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="766" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C766" s="22"/>
     </row>
-    <row r="767" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="767" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C767" s="22"/>
     </row>
-    <row r="768" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="768" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C768" s="22"/>
     </row>
-    <row r="769" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="769" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C769" s="22"/>
     </row>
-    <row r="770" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="770" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C770" s="22"/>
     </row>
-    <row r="771" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="771" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C771" s="22"/>
     </row>
-    <row r="772" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="772" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C772" s="22"/>
     </row>
-    <row r="773" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="773" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C773" s="22"/>
     </row>
-    <row r="774" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="774" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C774" s="22"/>
     </row>
-    <row r="775" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="775" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C775" s="22"/>
     </row>
-    <row r="776" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="776" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C776" s="22"/>
     </row>
-    <row r="777" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="777" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C777" s="22"/>
     </row>
-    <row r="778" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="778" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C778" s="22"/>
     </row>
-    <row r="779" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="779" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C779" s="22"/>
     </row>
-    <row r="780" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="780" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C780" s="22"/>
     </row>
-    <row r="781" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="781" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C781" s="22"/>
     </row>
-    <row r="782" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="782" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C782" s="22"/>
     </row>
-    <row r="783" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="783" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C783" s="22"/>
     </row>
-    <row r="784" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="784" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C784" s="22"/>
     </row>
-    <row r="785" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="785" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C785" s="22"/>
     </row>
-    <row r="786" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="786" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C786" s="22"/>
     </row>
-    <row r="787" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="787" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C787" s="22"/>
     </row>
-    <row r="788" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="788" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C788" s="22"/>
     </row>
-    <row r="789" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="789" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C789" s="22"/>
     </row>
-    <row r="790" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="790" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C790" s="22"/>
     </row>
-    <row r="791" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="791" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C791" s="22"/>
     </row>
-    <row r="792" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="792" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C792" s="22"/>
     </row>
-    <row r="793" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="793" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C793" s="22"/>
     </row>
-    <row r="794" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="794" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C794" s="22"/>
     </row>
-    <row r="795" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="795" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C795" s="22"/>
     </row>
-    <row r="796" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="796" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C796" s="22"/>
     </row>
-    <row r="797" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="797" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C797" s="22"/>
     </row>
-    <row r="798" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="798" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C798" s="22"/>
     </row>
-    <row r="799" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="799" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C799" s="22"/>
     </row>
-    <row r="800" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="800" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C800" s="22"/>
     </row>
-    <row r="801" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="801" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C801" s="22"/>
     </row>
-    <row r="802" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="802" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C802" s="22"/>
     </row>
-    <row r="803" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="803" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C803" s="22"/>
     </row>
-    <row r="804" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="804" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C804" s="22"/>
     </row>
-    <row r="805" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="805" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C805" s="22"/>
     </row>
-    <row r="806" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="806" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C806" s="22"/>
     </row>
-    <row r="807" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="807" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C807" s="22"/>
     </row>
-    <row r="808" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="808" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C808" s="22"/>
     </row>
-    <row r="809" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="809" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C809" s="22"/>
     </row>
-    <row r="810" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="810" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C810" s="22"/>
     </row>
-    <row r="811" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="811" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C811" s="22"/>
     </row>
-    <row r="812" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="812" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C812" s="22"/>
     </row>
-    <row r="813" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="813" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C813" s="22"/>
     </row>
-    <row r="814" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="814" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C814" s="22"/>
     </row>
-    <row r="815" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="815" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C815" s="22"/>
     </row>
-    <row r="816" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="816" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C816" s="22"/>
     </row>
-    <row r="817" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="817" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C817" s="22"/>
     </row>
-    <row r="818" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="818" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C818" s="22"/>
     </row>
-    <row r="819" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="819" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C819" s="22"/>
     </row>
-    <row r="820" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="820" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C820" s="22"/>
     </row>
-    <row r="821" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="821" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C821" s="22"/>
     </row>
-    <row r="822" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="822" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C822" s="22"/>
     </row>
-    <row r="823" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="823" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C823" s="22"/>
     </row>
-    <row r="824" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="824" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C824" s="22"/>
     </row>
-    <row r="825" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="825" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C825" s="22"/>
     </row>
-    <row r="826" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="826" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C826" s="22"/>
     </row>
-    <row r="827" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="827" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C827" s="22"/>
     </row>
-    <row r="828" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="828" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C828" s="22"/>
     </row>
-    <row r="829" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="829" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C829" s="22"/>
     </row>
-    <row r="830" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="830" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C830" s="22"/>
     </row>
-    <row r="831" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="831" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C831" s="22"/>
     </row>
-    <row r="832" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="832" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C832" s="22"/>
     </row>
-    <row r="833" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="833" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C833" s="22"/>
     </row>
-    <row r="834" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="834" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C834" s="22"/>
     </row>
-    <row r="835" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="835" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C835" s="22"/>
     </row>
-    <row r="836" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="836" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C836" s="22"/>
     </row>
-    <row r="837" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="837" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C837" s="22"/>
     </row>
-    <row r="838" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="838" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C838" s="22"/>
     </row>
-    <row r="839" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="839" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C839" s="22"/>
     </row>
-    <row r="840" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="840" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C840" s="22"/>
     </row>
-    <row r="841" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="841" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C841" s="22"/>
     </row>
-    <row r="842" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="842" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C842" s="22"/>
     </row>
-    <row r="843" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="843" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C843" s="22"/>
     </row>
-    <row r="844" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="844" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C844" s="22"/>
     </row>
-    <row r="845" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="845" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C845" s="22"/>
     </row>
-    <row r="846" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="846" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C846" s="22"/>
     </row>
-    <row r="847" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="847" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C847" s="22"/>
     </row>
-    <row r="848" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="848" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C848" s="22"/>
     </row>
-    <row r="849" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="849" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C849" s="22"/>
     </row>
-    <row r="850" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="850" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C850" s="22"/>
     </row>
-    <row r="851" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="851" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C851" s="22"/>
     </row>
-    <row r="852" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="852" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C852" s="22"/>
     </row>
-    <row r="853" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="853" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C853" s="22"/>
     </row>
-    <row r="854" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="854" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C854" s="22"/>
     </row>
-    <row r="855" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="855" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C855" s="22"/>
     </row>
-    <row r="856" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="856" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C856" s="22"/>
     </row>
-    <row r="857" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="857" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C857" s="22"/>
     </row>
-    <row r="858" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="858" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C858" s="22"/>
     </row>
-    <row r="859" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="859" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C859" s="22"/>
     </row>
-    <row r="860" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="860" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C860" s="22"/>
     </row>
-    <row r="861" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="861" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C861" s="22"/>
     </row>
-    <row r="862" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="862" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C862" s="22"/>
     </row>
-    <row r="863" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="863" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C863" s="22"/>
     </row>
-    <row r="864" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="864" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C864" s="22"/>
     </row>
-    <row r="865" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="865" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C865" s="22"/>
     </row>
-    <row r="866" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="866" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C866" s="22"/>
     </row>
-    <row r="867" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="867" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C867" s="22"/>
     </row>
-    <row r="868" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="868" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C868" s="22"/>
     </row>
-    <row r="869" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="869" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C869" s="22"/>
     </row>
-    <row r="870" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="870" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C870" s="22"/>
     </row>
-    <row r="871" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="871" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C871" s="22"/>
     </row>
-    <row r="872" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="872" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C872" s="22"/>
     </row>
-    <row r="873" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="873" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C873" s="22"/>
     </row>
-    <row r="874" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="874" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C874" s="22"/>
     </row>
-    <row r="875" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="875" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C875" s="22"/>
     </row>
-    <row r="876" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="876" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C876" s="22"/>
     </row>
-    <row r="877" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="877" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C877" s="22"/>
     </row>
-    <row r="878" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="878" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C878" s="22"/>
     </row>
-    <row r="879" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="879" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C879" s="22"/>
     </row>
-    <row r="880" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="880" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C880" s="22"/>
     </row>
-    <row r="881" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="881" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C881" s="22"/>
     </row>
-    <row r="882" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="882" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C882" s="22"/>
     </row>
-    <row r="883" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="883" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C883" s="22"/>
     </row>
-    <row r="884" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="884" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C884" s="22"/>
     </row>
-    <row r="885" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="885" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C885" s="22"/>
     </row>
-    <row r="886" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="886" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C886" s="22"/>
     </row>
-    <row r="887" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="887" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C887" s="22"/>
     </row>
-    <row r="888" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="888" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C888" s="22"/>
     </row>
-    <row r="889" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="889" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C889" s="22"/>
     </row>
-    <row r="890" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="890" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C890" s="22"/>
     </row>
-    <row r="891" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="891" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C891" s="22"/>
     </row>
-    <row r="892" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="892" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C892" s="22"/>
     </row>
-    <row r="893" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="893" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C893" s="22"/>
     </row>
-    <row r="894" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="894" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C894" s="22"/>
     </row>
-    <row r="895" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="895" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C895" s="22"/>
     </row>
-    <row r="896" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="896" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C896" s="22"/>
     </row>
-    <row r="897" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="897" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C897" s="22"/>
     </row>
-    <row r="898" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="898" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C898" s="22"/>
     </row>
-    <row r="899" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="899" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C899" s="22"/>
     </row>
-    <row r="900" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="900" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C900" s="22"/>
     </row>
-    <row r="901" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="901" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C901" s="22"/>
     </row>
-    <row r="902" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="902" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C902" s="22"/>
     </row>
-    <row r="903" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="903" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C903" s="22"/>
     </row>
-    <row r="904" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="904" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C904" s="22"/>
     </row>
-    <row r="905" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="905" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C905" s="22"/>
     </row>
-    <row r="906" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="906" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C906" s="22"/>
     </row>
-    <row r="907" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="907" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C907" s="22"/>
     </row>
-    <row r="908" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="908" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C908" s="22"/>
     </row>
-    <row r="909" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="909" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C909" s="22"/>
     </row>
-    <row r="910" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="910" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C910" s="22"/>
     </row>
-    <row r="911" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="911" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C911" s="22"/>
     </row>
-    <row r="912" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="912" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C912" s="22"/>
     </row>
-    <row r="913" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="913" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C913" s="22"/>
     </row>
-    <row r="914" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="914" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C914" s="22"/>
     </row>
-    <row r="915" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="915" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C915" s="22"/>
     </row>
-    <row r="916" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="916" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C916" s="22"/>
     </row>
-    <row r="917" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="917" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C917" s="22"/>
     </row>
-    <row r="918" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="918" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C918" s="22"/>
     </row>
-    <row r="919" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="919" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C919" s="22"/>
     </row>
-    <row r="920" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="920" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C920" s="22"/>
     </row>
-    <row r="921" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="921" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C921" s="22"/>
     </row>
-    <row r="922" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="922" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C922" s="22"/>
     </row>
-    <row r="923" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="923" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C923" s="22"/>
     </row>
-    <row r="924" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="924" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C924" s="22"/>
     </row>
-    <row r="925" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="925" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C925" s="22"/>
     </row>
-    <row r="926" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="926" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C926" s="22"/>
     </row>
-    <row r="927" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="927" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C927" s="22"/>
     </row>
-    <row r="928" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="928" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C928" s="22"/>
     </row>
-    <row r="929" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="929" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C929" s="22"/>
     </row>
-    <row r="930" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="930" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C930" s="22"/>
     </row>
-    <row r="931" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="931" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C931" s="22"/>
     </row>
-    <row r="932" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="932" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C932" s="22"/>
     </row>
-    <row r="933" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="933" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C933" s="22"/>
     </row>
-    <row r="934" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="934" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C934" s="22"/>
     </row>
-    <row r="935" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="935" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C935" s="22"/>
     </row>
-    <row r="936" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="936" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C936" s="22"/>
     </row>
-    <row r="937" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="937" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C937" s="22"/>
     </row>
-    <row r="938" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="938" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C938" s="22"/>
     </row>
-    <row r="939" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="939" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C939" s="22"/>
     </row>
-    <row r="940" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="940" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C940" s="22"/>
     </row>
-    <row r="941" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="941" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C941" s="22"/>
     </row>
-    <row r="942" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="942" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C942" s="22"/>
     </row>
-    <row r="943" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="943" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C943" s="22"/>
     </row>
-    <row r="944" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="944" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C944" s="22"/>
     </row>
-    <row r="945" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="945" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C945" s="22"/>
     </row>
-    <row r="946" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="946" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C946" s="22"/>
     </row>
-    <row r="947" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="947" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C947" s="22"/>
     </row>
-    <row r="948" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="948" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C948" s="22"/>
     </row>
-    <row r="949" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="949" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C949" s="22"/>
     </row>
-    <row r="950" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="950" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C950" s="22"/>
     </row>
-    <row r="951" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="951" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C951" s="22"/>
     </row>
-    <row r="952" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="952" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C952" s="22"/>
     </row>
-    <row r="953" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="953" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C953" s="22"/>
     </row>
-    <row r="954" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="954" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C954" s="22"/>
     </row>
-    <row r="955" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="955" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C955" s="22"/>
     </row>
-    <row r="956" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="956" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C956" s="22"/>
     </row>
-    <row r="957" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="957" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C957" s="22"/>
     </row>
-    <row r="958" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="958" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C958" s="22"/>
     </row>
-    <row r="959" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="959" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C959" s="22"/>
     </row>
-    <row r="960" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="960" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C960" s="22"/>
     </row>
-    <row r="961" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="961" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C961" s="22"/>
     </row>
-    <row r="962" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="962" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C962" s="22"/>
     </row>
-    <row r="963" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="963" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C963" s="22"/>
     </row>
-    <row r="964" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="964" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C964" s="22"/>
     </row>
-    <row r="965" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="965" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C965" s="22"/>
     </row>
-    <row r="966" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="966" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C966" s="22"/>
     </row>
-    <row r="967" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="967" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C967" s="22"/>
     </row>
-    <row r="968" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="968" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C968" s="22"/>
     </row>
-    <row r="969" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="969" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C969" s="22"/>
     </row>
-    <row r="970" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="970" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C970" s="22"/>
     </row>
-    <row r="971" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="971" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C971" s="22"/>
     </row>
-    <row r="972" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="972" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C972" s="22"/>
     </row>
-    <row r="973" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="973" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C973" s="22"/>
     </row>
-    <row r="974" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="974" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C974" s="22"/>
     </row>
-    <row r="975" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="975" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C975" s="22"/>
     </row>
-    <row r="976" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="976" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C976" s="22"/>
     </row>
-    <row r="977" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="977" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C977" s="22"/>
     </row>
-    <row r="978" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="978" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C978" s="22"/>
     </row>
-    <row r="979" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="979" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C979" s="22"/>
     </row>
-    <row r="980" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="980" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C980" s="22"/>
     </row>
-    <row r="981" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="981" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C981" s="22"/>
     </row>
-    <row r="982" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="982" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C982" s="22"/>
     </row>
-    <row r="983" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="983" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C983" s="22"/>
     </row>
-    <row r="984" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="984" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C984" s="22"/>
     </row>
-    <row r="985" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="985" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C985" s="22"/>
     </row>
-    <row r="986" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="986" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C986" s="22"/>
     </row>
-    <row r="987" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="987" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C987" s="22"/>
     </row>
-    <row r="988" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="988" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C988" s="22"/>
     </row>
-    <row r="989" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="989" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C989" s="22"/>
     </row>
-    <row r="990" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="990" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C990" s="22"/>
     </row>
-    <row r="991" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="991" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C991" s="22"/>
     </row>
-    <row r="992" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="992" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C992" s="22"/>
     </row>
-    <row r="993" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="993" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C993" s="22"/>
     </row>
-    <row r="994" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="994" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C994" s="22"/>
     </row>
-    <row r="995" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="995" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C995" s="22"/>
     </row>
-    <row r="996" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="996" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C996" s="22"/>
     </row>
-    <row r="997" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="997" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C997" s="22"/>
     </row>
-    <row r="998" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="998" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C998" s="22"/>
     </row>
-    <row r="999" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="999" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C999" s="22"/>
     </row>
-    <row r="1000" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1000" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1000" s="22"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed Set_Matrix_Zeroes & created tutorial image
</commit_message>
<xml_diff>
--- a/Leetcode 75.xlsx
+++ b/Leetcode 75.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christianm\Desktop\Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D02DC5D-C1CD-4D76-AA9A-A46B3524C0D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6A4834-2070-4F03-BD69-11D6282ABF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="318">
   <si>
     <t>Video Solution</t>
   </si>
@@ -1505,8 +1505,8 @@
   </sheetPr>
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2430,7 +2430,9 @@
       <c r="B47" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="C47" s="18"/>
+      <c r="C47" s="24" t="s">
+        <v>8</v>
+      </c>
       <c r="D47" s="10" t="s">
         <v>195</v>
       </c>

</xml_diff>

<commit_message>
Completed top k frequent elements
</commit_message>
<xml_diff>
--- a/Leetcode 75.xlsx
+++ b/Leetcode 75.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christianm\Desktop\Learning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christianm\PycharmProjects\DSA_and_Leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFB5168-387A-456A-850C-1AF74954C0D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD51A8A1-40AA-4DF5-AA68-AA460DC4B259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="318">
   <si>
     <t>Video Solution</t>
   </si>
@@ -1508,21 +1508,21 @@
   </sheetPr>
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" customWidth="1"/>
-    <col min="4" max="4" width="57.140625" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" customWidth="1"/>
-    <col min="6" max="6" width="182.7109375" customWidth="1"/>
+    <col min="1" max="1" width="5.453125" customWidth="1"/>
+    <col min="2" max="2" width="18.7265625" customWidth="1"/>
+    <col min="3" max="3" width="7.1796875" customWidth="1"/>
+    <col min="4" max="4" width="57.1796875" customWidth="1"/>
+    <col min="5" max="5" width="31.81640625" customWidth="1"/>
+    <col min="6" max="6" width="182.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>20</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>24</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>28</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>36</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>40</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>44</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>48</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>53</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>57</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>61</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>65</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>69</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>74</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>78</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>82</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>86</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>90</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>94</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>98</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>102</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>106</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>110</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>114</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>119</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>123</v>
       </c>
@@ -2118,7 +2118,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>127</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>131</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="16" t="s">
         <v>135</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="16" t="s">
         <v>139</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="16" t="s">
         <v>143</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>147</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>152</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>156</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>160</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="19" t="s">
         <v>164</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>168</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>173</v>
       </c>
@@ -2352,7 +2352,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>177</v>
       </c>
@@ -2372,7 +2372,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>181</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>185</v>
       </c>
@@ -2412,7 +2412,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>189</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>193</v>
       </c>
@@ -2452,7 +2452,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>198</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>202</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>206</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>210</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
         <v>215</v>
       </c>
@@ -2552,7 +2552,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="21" t="s">
         <v>219</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
         <v>223</v>
       </c>
@@ -2592,7 +2592,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
         <v>227</v>
       </c>
@@ -2612,7 +2612,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>231</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>235</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>239</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>243</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="16" t="s">
         <v>247</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
         <v>251</v>
       </c>
@@ -2732,7 +2732,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>256</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
         <v>260</v>
       </c>
@@ -2772,7 +2772,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>264</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
         <v>268</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>272</v>
       </c>
@@ -2828,7 +2828,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
         <v>276</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>280</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>284</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
         <v>288</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
         <v>292</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
         <v>296</v>
       </c>
@@ -2948,7 +2948,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
         <v>300</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
         <v>304</v>
       </c>
@@ -2988,7 +2988,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
         <v>181</v>
       </c>
@@ -3006,14 +3006,16 @@
         <v>309</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
         <v>310</v>
       </c>
       <c r="B76" s="6" t="s">
         <v>308</v>
       </c>
-      <c r="C76" s="13"/>
+      <c r="C76" s="25" t="s">
+        <v>8</v>
+      </c>
       <c r="D76" s="10" t="s">
         <v>311</v>
       </c>
@@ -3024,7 +3026,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="5" t="s">
         <v>314</v>
       </c>
@@ -3042,2973 +3044,2973 @@
         <v>317</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C78" s="22"/>
     </row>
-    <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C79" s="22"/>
     </row>
-    <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="23"/>
       <c r="C80" s="22"/>
     </row>
-    <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="23"/>
       <c r="C81" s="22"/>
     </row>
-    <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="23"/>
       <c r="C82" s="22"/>
     </row>
-    <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="23"/>
       <c r="C83" s="22"/>
     </row>
-    <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="23"/>
       <c r="C84" s="22"/>
     </row>
-    <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="23"/>
       <c r="C85" s="22"/>
     </row>
-    <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="23"/>
       <c r="C86" s="22"/>
     </row>
-    <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="23"/>
       <c r="C87" s="22"/>
     </row>
-    <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="23"/>
       <c r="C88" s="22"/>
     </row>
-    <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="23"/>
       <c r="C89" s="22"/>
     </row>
-    <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="23"/>
       <c r="C90" s="22"/>
     </row>
-    <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="23"/>
       <c r="C91" s="22"/>
     </row>
-    <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="23"/>
       <c r="C92" s="22"/>
     </row>
-    <row r="93" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="23"/>
       <c r="C93" s="22"/>
     </row>
-    <row r="94" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="23"/>
       <c r="C94" s="22"/>
     </row>
-    <row r="95" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="23"/>
       <c r="C95" s="22"/>
     </row>
-    <row r="96" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="23"/>
       <c r="C96" s="22"/>
     </row>
-    <row r="97" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="23"/>
       <c r="C97" s="22"/>
     </row>
-    <row r="98" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="23"/>
       <c r="C98" s="22"/>
     </row>
-    <row r="99" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="23"/>
       <c r="C99" s="22"/>
     </row>
-    <row r="100" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="23"/>
       <c r="C100" s="22"/>
     </row>
-    <row r="101" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="23"/>
       <c r="C101" s="22"/>
     </row>
-    <row r="102" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="23"/>
       <c r="C102" s="22"/>
     </row>
-    <row r="103" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="23"/>
       <c r="C103" s="22"/>
     </row>
-    <row r="104" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="23"/>
       <c r="C104" s="22"/>
     </row>
-    <row r="105" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="23"/>
       <c r="C105" s="22"/>
     </row>
-    <row r="106" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="23"/>
       <c r="C106" s="22"/>
     </row>
-    <row r="107" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="23"/>
       <c r="C107" s="22"/>
     </row>
-    <row r="108" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="23"/>
       <c r="C108" s="22"/>
     </row>
-    <row r="109" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="23"/>
       <c r="C109" s="22"/>
     </row>
-    <row r="110" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="23"/>
       <c r="C110" s="22"/>
     </row>
-    <row r="111" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="23"/>
       <c r="C111" s="22"/>
     </row>
-    <row r="112" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="23"/>
       <c r="C112" s="22"/>
     </row>
-    <row r="113" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="23"/>
       <c r="C113" s="22"/>
     </row>
-    <row r="114" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="23"/>
       <c r="C114" s="22"/>
     </row>
-    <row r="115" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="23"/>
       <c r="C115" s="22"/>
     </row>
-    <row r="116" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="23"/>
       <c r="C116" s="22"/>
     </row>
-    <row r="117" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="23"/>
       <c r="C117" s="22"/>
     </row>
-    <row r="118" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="23"/>
       <c r="C118" s="22"/>
     </row>
-    <row r="119" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="23"/>
       <c r="C119" s="22"/>
     </row>
-    <row r="120" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="23"/>
       <c r="C120" s="22"/>
     </row>
-    <row r="121" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="23"/>
       <c r="C121" s="22"/>
     </row>
-    <row r="122" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="23"/>
       <c r="C122" s="22"/>
     </row>
-    <row r="123" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="23"/>
       <c r="C123" s="22"/>
     </row>
-    <row r="124" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="23"/>
       <c r="C124" s="22"/>
     </row>
-    <row r="125" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="23"/>
       <c r="C125" s="22"/>
     </row>
-    <row r="126" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="23"/>
       <c r="C126" s="22"/>
     </row>
-    <row r="127" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="23"/>
       <c r="C127" s="22"/>
     </row>
-    <row r="128" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="23"/>
       <c r="C128" s="22"/>
     </row>
-    <row r="129" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="23"/>
       <c r="C129" s="22"/>
     </row>
-    <row r="130" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="23"/>
       <c r="C130" s="22"/>
     </row>
-    <row r="131" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="23"/>
       <c r="C131" s="22"/>
     </row>
-    <row r="132" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="23"/>
       <c r="C132" s="22"/>
     </row>
-    <row r="133" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="23"/>
       <c r="C133" s="22"/>
     </row>
-    <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="23"/>
       <c r="C134" s="22"/>
     </row>
-    <row r="135" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="23"/>
       <c r="C135" s="22"/>
     </row>
-    <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="23"/>
       <c r="C136" s="22"/>
     </row>
-    <row r="137" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="23"/>
       <c r="C137" s="22"/>
     </row>
-    <row r="138" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="23"/>
       <c r="C138" s="22"/>
     </row>
-    <row r="139" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="23"/>
       <c r="C139" s="22"/>
     </row>
-    <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="23"/>
       <c r="C140" s="22"/>
     </row>
-    <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="23"/>
       <c r="C141" s="22"/>
     </row>
-    <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="23"/>
       <c r="C142" s="22"/>
     </row>
-    <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="23"/>
       <c r="C143" s="22"/>
     </row>
-    <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="23"/>
       <c r="C144" s="22"/>
     </row>
-    <row r="145" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="23"/>
       <c r="C145" s="22"/>
     </row>
-    <row r="146" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="23"/>
       <c r="C146" s="22"/>
     </row>
-    <row r="147" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="23"/>
       <c r="C147" s="22"/>
     </row>
-    <row r="148" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="23"/>
       <c r="C148" s="22"/>
     </row>
-    <row r="149" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="23"/>
       <c r="C149" s="22"/>
     </row>
-    <row r="150" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="23"/>
       <c r="C150" s="22"/>
     </row>
-    <row r="151" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="23"/>
       <c r="C151" s="22"/>
     </row>
-    <row r="152" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="23"/>
       <c r="C152" s="22"/>
     </row>
-    <row r="153" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="23"/>
       <c r="C153" s="22"/>
     </row>
-    <row r="154" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="23"/>
       <c r="C154" s="22"/>
     </row>
-    <row r="155" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="23"/>
       <c r="C155" s="22"/>
     </row>
-    <row r="156" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="23"/>
       <c r="C156" s="22"/>
     </row>
-    <row r="157" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="23"/>
       <c r="C157" s="22"/>
     </row>
-    <row r="158" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="23"/>
       <c r="C158" s="22"/>
     </row>
-    <row r="159" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="23"/>
       <c r="C159" s="22"/>
     </row>
-    <row r="160" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="23"/>
       <c r="C160" s="22"/>
     </row>
-    <row r="161" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="23"/>
       <c r="C161" s="22"/>
     </row>
-    <row r="162" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="23"/>
       <c r="C162" s="22"/>
     </row>
-    <row r="163" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="23"/>
       <c r="C163" s="22"/>
     </row>
-    <row r="164" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="23"/>
       <c r="C164" s="22"/>
     </row>
-    <row r="165" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="23"/>
       <c r="C165" s="22"/>
     </row>
-    <row r="166" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="23"/>
       <c r="C166" s="22"/>
     </row>
-    <row r="167" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="23"/>
       <c r="C167" s="22"/>
     </row>
-    <row r="168" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="23"/>
       <c r="C168" s="22"/>
     </row>
-    <row r="169" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="23"/>
       <c r="C169" s="22"/>
     </row>
-    <row r="170" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="23"/>
       <c r="C170" s="22"/>
     </row>
-    <row r="171" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="23"/>
       <c r="C171" s="22"/>
     </row>
-    <row r="172" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="23"/>
       <c r="C172" s="22"/>
     </row>
-    <row r="173" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="23"/>
       <c r="C173" s="22"/>
     </row>
-    <row r="174" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="23"/>
       <c r="C174" s="22"/>
     </row>
-    <row r="175" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="23"/>
       <c r="C175" s="22"/>
     </row>
-    <row r="176" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="23"/>
       <c r="C176" s="22"/>
     </row>
-    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="23"/>
       <c r="C177" s="22"/>
     </row>
-    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="23"/>
       <c r="C178" s="22"/>
     </row>
-    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="23"/>
       <c r="C179" s="22"/>
     </row>
-    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="23"/>
       <c r="C180" s="22"/>
     </row>
-    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="23"/>
       <c r="C181" s="22"/>
     </row>
-    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="23"/>
       <c r="C182" s="22"/>
     </row>
-    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="23"/>
       <c r="C183" s="22"/>
     </row>
-    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A184" s="23"/>
       <c r="C184" s="22"/>
     </row>
-    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="23"/>
       <c r="C185" s="22"/>
     </row>
-    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A186" s="23"/>
       <c r="C186" s="22"/>
     </row>
-    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A187" s="23"/>
       <c r="C187" s="22"/>
     </row>
-    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A188" s="23"/>
       <c r="C188" s="22"/>
     </row>
-    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A189" s="23"/>
       <c r="C189" s="22"/>
     </row>
-    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A190" s="23"/>
       <c r="C190" s="22"/>
     </row>
-    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A191" s="23"/>
       <c r="C191" s="22"/>
     </row>
-    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A192" s="23"/>
       <c r="C192" s="22"/>
     </row>
-    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A193" s="23"/>
       <c r="C193" s="22"/>
     </row>
-    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A194" s="23"/>
       <c r="C194" s="22"/>
     </row>
-    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A195" s="23"/>
       <c r="C195" s="22"/>
     </row>
-    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A196" s="23"/>
       <c r="C196" s="22"/>
     </row>
-    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A197" s="23"/>
       <c r="C197" s="22"/>
     </row>
-    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A198" s="23"/>
       <c r="C198" s="22"/>
     </row>
-    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A199" s="23"/>
       <c r="C199" s="22"/>
     </row>
-    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A200" s="23"/>
       <c r="C200" s="22"/>
     </row>
-    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A201" s="23"/>
       <c r="C201" s="22"/>
     </row>
-    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A202" s="23"/>
       <c r="C202" s="22"/>
     </row>
-    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A203" s="23"/>
       <c r="C203" s="22"/>
     </row>
-    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A204" s="23"/>
       <c r="C204" s="22"/>
     </row>
-    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A205" s="23"/>
       <c r="C205" s="22"/>
     </row>
-    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A206" s="23"/>
       <c r="C206" s="22"/>
     </row>
-    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A207" s="23"/>
       <c r="C207" s="22"/>
     </row>
-    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A208" s="23"/>
       <c r="C208" s="22"/>
     </row>
-    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A209" s="23"/>
       <c r="C209" s="22"/>
     </row>
-    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A210" s="23"/>
       <c r="C210" s="22"/>
     </row>
-    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A211" s="23"/>
       <c r="C211" s="22"/>
     </row>
-    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A212" s="23"/>
       <c r="C212" s="22"/>
     </row>
-    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A213" s="23"/>
       <c r="C213" s="22"/>
     </row>
-    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A214" s="23"/>
       <c r="C214" s="22"/>
     </row>
-    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A215" s="23"/>
       <c r="C215" s="22"/>
     </row>
-    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A216" s="23"/>
       <c r="C216" s="22"/>
     </row>
-    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A217" s="23"/>
       <c r="C217" s="22"/>
     </row>
-    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A218" s="23"/>
       <c r="C218" s="22"/>
     </row>
-    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A219" s="23"/>
       <c r="C219" s="22"/>
     </row>
-    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A220" s="23"/>
       <c r="C220" s="22"/>
     </row>
-    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A221" s="23"/>
       <c r="C221" s="22"/>
     </row>
-    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="23"/>
       <c r="C222" s="22"/>
     </row>
-    <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A223" s="23"/>
       <c r="C223" s="22"/>
     </row>
-    <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A224" s="23"/>
       <c r="C224" s="22"/>
     </row>
-    <row r="225" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A225" s="23"/>
       <c r="C225" s="22"/>
     </row>
-    <row r="226" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A226" s="23"/>
       <c r="C226" s="22"/>
     </row>
-    <row r="227" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A227" s="23"/>
       <c r="C227" s="22"/>
     </row>
-    <row r="228" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A228" s="23"/>
       <c r="C228" s="22"/>
     </row>
-    <row r="229" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A229" s="23"/>
       <c r="C229" s="22"/>
     </row>
-    <row r="230" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A230" s="23"/>
       <c r="C230" s="22"/>
     </row>
-    <row r="231" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A231" s="23"/>
       <c r="C231" s="22"/>
     </row>
-    <row r="232" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A232" s="23"/>
       <c r="C232" s="22"/>
     </row>
-    <row r="233" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A233" s="23"/>
       <c r="C233" s="22"/>
     </row>
-    <row r="234" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A234" s="23"/>
       <c r="C234" s="22"/>
     </row>
-    <row r="235" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A235" s="23"/>
       <c r="C235" s="22"/>
     </row>
-    <row r="236" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="23"/>
       <c r="C236" s="22"/>
     </row>
-    <row r="237" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A237" s="23"/>
       <c r="C237" s="22"/>
     </row>
-    <row r="238" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A238" s="23"/>
       <c r="C238" s="22"/>
     </row>
-    <row r="239" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A239" s="23"/>
       <c r="C239" s="22"/>
     </row>
-    <row r="240" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A240" s="23"/>
       <c r="C240" s="22"/>
     </row>
-    <row r="241" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A241" s="23"/>
       <c r="C241" s="22"/>
     </row>
-    <row r="242" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A242" s="23"/>
       <c r="C242" s="22"/>
     </row>
-    <row r="243" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A243" s="23"/>
       <c r="C243" s="22"/>
     </row>
-    <row r="244" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A244" s="23"/>
       <c r="C244" s="22"/>
     </row>
-    <row r="245" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A245" s="23"/>
       <c r="C245" s="22"/>
     </row>
-    <row r="246" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A246" s="23"/>
       <c r="C246" s="22"/>
     </row>
-    <row r="247" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A247" s="23"/>
       <c r="C247" s="22"/>
     </row>
-    <row r="248" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A248" s="23"/>
       <c r="C248" s="22"/>
     </row>
-    <row r="249" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A249" s="23"/>
       <c r="C249" s="22"/>
     </row>
-    <row r="250" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A250" s="23"/>
       <c r="C250" s="22"/>
     </row>
-    <row r="251" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A251" s="23"/>
       <c r="C251" s="22"/>
     </row>
-    <row r="252" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A252" s="23"/>
       <c r="C252" s="22"/>
     </row>
-    <row r="253" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A253" s="23"/>
       <c r="C253" s="22"/>
     </row>
-    <row r="254" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A254" s="23"/>
       <c r="C254" s="22"/>
     </row>
-    <row r="255" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A255" s="23"/>
       <c r="C255" s="22"/>
     </row>
-    <row r="256" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A256" s="23"/>
       <c r="C256" s="22"/>
     </row>
-    <row r="257" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A257" s="23"/>
       <c r="C257" s="22"/>
     </row>
-    <row r="258" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A258" s="23"/>
       <c r="C258" s="22"/>
     </row>
-    <row r="259" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A259" s="23"/>
       <c r="C259" s="22"/>
     </row>
-    <row r="260" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A260" s="23"/>
       <c r="C260" s="22"/>
     </row>
-    <row r="261" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A261" s="23"/>
       <c r="C261" s="22"/>
     </row>
-    <row r="262" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A262" s="23"/>
       <c r="C262" s="22"/>
     </row>
-    <row r="263" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A263" s="23"/>
       <c r="C263" s="22"/>
     </row>
-    <row r="264" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A264" s="23"/>
       <c r="C264" s="22"/>
     </row>
-    <row r="265" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A265" s="23"/>
       <c r="C265" s="22"/>
     </row>
-    <row r="266" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A266" s="23"/>
       <c r="C266" s="22"/>
     </row>
-    <row r="267" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A267" s="23"/>
       <c r="C267" s="22"/>
     </row>
-    <row r="268" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A268" s="23"/>
       <c r="C268" s="22"/>
     </row>
-    <row r="269" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A269" s="23"/>
       <c r="C269" s="22"/>
     </row>
-    <row r="270" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A270" s="23"/>
       <c r="C270" s="22"/>
     </row>
-    <row r="271" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A271" s="23"/>
       <c r="C271" s="22"/>
     </row>
-    <row r="272" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A272" s="23"/>
       <c r="C272" s="22"/>
     </row>
-    <row r="273" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A273" s="23"/>
       <c r="C273" s="22"/>
     </row>
-    <row r="274" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A274" s="23"/>
       <c r="C274" s="22"/>
     </row>
-    <row r="275" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A275" s="23"/>
       <c r="C275" s="22"/>
     </row>
-    <row r="276" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A276" s="23"/>
       <c r="C276" s="22"/>
     </row>
-    <row r="277" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A277" s="23"/>
       <c r="C277" s="22"/>
     </row>
-    <row r="278" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A278" s="23"/>
       <c r="C278" s="22"/>
     </row>
-    <row r="279" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A279" s="23"/>
       <c r="C279" s="22"/>
     </row>
-    <row r="280" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C280" s="22"/>
     </row>
-    <row r="281" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C281" s="22"/>
     </row>
-    <row r="282" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C282" s="22"/>
     </row>
-    <row r="283" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C283" s="22"/>
     </row>
-    <row r="284" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C284" s="22"/>
     </row>
-    <row r="285" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C285" s="22"/>
     </row>
-    <row r="286" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C286" s="22"/>
     </row>
-    <row r="287" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C287" s="22"/>
     </row>
-    <row r="288" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C288" s="22"/>
     </row>
-    <row r="289" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C289" s="22"/>
     </row>
-    <row r="290" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C290" s="22"/>
     </row>
-    <row r="291" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C291" s="22"/>
     </row>
-    <row r="292" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C292" s="22"/>
     </row>
-    <row r="293" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C293" s="22"/>
     </row>
-    <row r="294" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C294" s="22"/>
     </row>
-    <row r="295" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C295" s="22"/>
     </row>
-    <row r="296" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C296" s="22"/>
     </row>
-    <row r="297" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C297" s="22"/>
     </row>
-    <row r="298" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C298" s="22"/>
     </row>
-    <row r="299" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C299" s="22"/>
     </row>
-    <row r="300" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C300" s="22"/>
     </row>
-    <row r="301" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C301" s="22"/>
     </row>
-    <row r="302" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C302" s="22"/>
     </row>
-    <row r="303" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C303" s="22"/>
     </row>
-    <row r="304" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C304" s="22"/>
     </row>
-    <row r="305" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C305" s="22"/>
     </row>
-    <row r="306" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C306" s="22"/>
     </row>
-    <row r="307" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C307" s="22"/>
     </row>
-    <row r="308" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C308" s="22"/>
     </row>
-    <row r="309" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C309" s="22"/>
     </row>
-    <row r="310" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C310" s="22"/>
     </row>
-    <row r="311" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C311" s="22"/>
     </row>
-    <row r="312" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C312" s="22"/>
     </row>
-    <row r="313" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C313" s="22"/>
     </row>
-    <row r="314" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C314" s="22"/>
     </row>
-    <row r="315" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C315" s="22"/>
     </row>
-    <row r="316" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C316" s="22"/>
     </row>
-    <row r="317" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C317" s="22"/>
     </row>
-    <row r="318" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C318" s="22"/>
     </row>
-    <row r="319" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C319" s="22"/>
     </row>
-    <row r="320" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C320" s="22"/>
     </row>
-    <row r="321" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C321" s="22"/>
     </row>
-    <row r="322" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C322" s="22"/>
     </row>
-    <row r="323" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C323" s="22"/>
     </row>
-    <row r="324" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C324" s="22"/>
     </row>
-    <row r="325" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C325" s="22"/>
     </row>
-    <row r="326" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C326" s="22"/>
     </row>
-    <row r="327" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C327" s="22"/>
     </row>
-    <row r="328" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C328" s="22"/>
     </row>
-    <row r="329" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C329" s="22"/>
     </row>
-    <row r="330" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C330" s="22"/>
     </row>
-    <row r="331" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C331" s="22"/>
     </row>
-    <row r="332" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C332" s="22"/>
     </row>
-    <row r="333" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C333" s="22"/>
     </row>
-    <row r="334" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C334" s="22"/>
     </row>
-    <row r="335" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="335" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C335" s="22"/>
     </row>
-    <row r="336" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C336" s="22"/>
     </row>
-    <row r="337" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="337" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C337" s="22"/>
     </row>
-    <row r="338" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C338" s="22"/>
     </row>
-    <row r="339" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C339" s="22"/>
     </row>
-    <row r="340" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C340" s="22"/>
     </row>
-    <row r="341" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C341" s="22"/>
     </row>
-    <row r="342" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="342" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C342" s="22"/>
     </row>
-    <row r="343" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="343" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C343" s="22"/>
     </row>
-    <row r="344" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="344" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C344" s="22"/>
     </row>
-    <row r="345" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="345" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C345" s="22"/>
     </row>
-    <row r="346" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="346" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C346" s="22"/>
     </row>
-    <row r="347" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="347" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C347" s="22"/>
     </row>
-    <row r="348" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="348" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C348" s="22"/>
     </row>
-    <row r="349" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="349" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C349" s="22"/>
     </row>
-    <row r="350" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="350" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C350" s="22"/>
     </row>
-    <row r="351" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="351" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C351" s="22"/>
     </row>
-    <row r="352" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="352" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C352" s="22"/>
     </row>
-    <row r="353" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="353" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C353" s="22"/>
     </row>
-    <row r="354" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="354" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C354" s="22"/>
     </row>
-    <row r="355" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="355" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C355" s="22"/>
     </row>
-    <row r="356" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="356" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C356" s="22"/>
     </row>
-    <row r="357" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="357" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C357" s="22"/>
     </row>
-    <row r="358" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="358" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C358" s="22"/>
     </row>
-    <row r="359" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="359" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C359" s="22"/>
     </row>
-    <row r="360" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="360" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C360" s="22"/>
     </row>
-    <row r="361" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="361" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C361" s="22"/>
     </row>
-    <row r="362" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="362" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C362" s="22"/>
     </row>
-    <row r="363" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="363" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C363" s="22"/>
     </row>
-    <row r="364" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="364" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C364" s="22"/>
     </row>
-    <row r="365" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="365" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C365" s="22"/>
     </row>
-    <row r="366" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="366" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C366" s="22"/>
     </row>
-    <row r="367" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="367" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C367" s="22"/>
     </row>
-    <row r="368" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="368" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C368" s="22"/>
     </row>
-    <row r="369" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="369" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C369" s="22"/>
     </row>
-    <row r="370" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="370" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C370" s="22"/>
     </row>
-    <row r="371" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="371" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C371" s="22"/>
     </row>
-    <row r="372" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="372" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C372" s="22"/>
     </row>
-    <row r="373" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="373" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C373" s="22"/>
     </row>
-    <row r="374" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="374" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C374" s="22"/>
     </row>
-    <row r="375" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="375" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C375" s="22"/>
     </row>
-    <row r="376" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="376" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C376" s="22"/>
     </row>
-    <row r="377" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="377" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C377" s="22"/>
     </row>
-    <row r="378" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="378" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C378" s="22"/>
     </row>
-    <row r="379" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="379" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C379" s="22"/>
     </row>
-    <row r="380" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="380" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C380" s="22"/>
     </row>
-    <row r="381" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="381" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C381" s="22"/>
     </row>
-    <row r="382" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="382" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C382" s="22"/>
     </row>
-    <row r="383" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="383" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C383" s="22"/>
     </row>
-    <row r="384" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="384" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C384" s="22"/>
     </row>
-    <row r="385" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="385" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C385" s="22"/>
     </row>
-    <row r="386" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="386" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C386" s="22"/>
     </row>
-    <row r="387" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="387" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C387" s="22"/>
     </row>
-    <row r="388" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="388" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C388" s="22"/>
     </row>
-    <row r="389" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="389" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C389" s="22"/>
     </row>
-    <row r="390" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="390" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C390" s="22"/>
     </row>
-    <row r="391" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="391" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C391" s="22"/>
     </row>
-    <row r="392" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="392" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C392" s="22"/>
     </row>
-    <row r="393" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="393" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C393" s="22"/>
     </row>
-    <row r="394" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="394" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C394" s="22"/>
     </row>
-    <row r="395" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="395" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C395" s="22"/>
     </row>
-    <row r="396" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="396" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C396" s="22"/>
     </row>
-    <row r="397" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="397" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C397" s="22"/>
     </row>
-    <row r="398" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="398" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C398" s="22"/>
     </row>
-    <row r="399" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="399" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C399" s="22"/>
     </row>
-    <row r="400" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="400" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C400" s="22"/>
     </row>
-    <row r="401" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="401" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C401" s="22"/>
     </row>
-    <row r="402" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="402" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C402" s="22"/>
     </row>
-    <row r="403" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="403" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C403" s="22"/>
     </row>
-    <row r="404" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="404" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C404" s="22"/>
     </row>
-    <row r="405" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="405" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C405" s="22"/>
     </row>
-    <row r="406" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="406" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C406" s="22"/>
     </row>
-    <row r="407" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="407" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C407" s="22"/>
     </row>
-    <row r="408" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="408" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C408" s="22"/>
     </row>
-    <row r="409" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="409" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C409" s="22"/>
     </row>
-    <row r="410" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="410" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C410" s="22"/>
     </row>
-    <row r="411" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="411" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C411" s="22"/>
     </row>
-    <row r="412" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="412" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C412" s="22"/>
     </row>
-    <row r="413" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="413" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C413" s="22"/>
     </row>
-    <row r="414" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="414" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C414" s="22"/>
     </row>
-    <row r="415" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="415" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C415" s="22"/>
     </row>
-    <row r="416" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="416" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C416" s="22"/>
     </row>
-    <row r="417" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="417" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C417" s="22"/>
     </row>
-    <row r="418" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="418" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C418" s="22"/>
     </row>
-    <row r="419" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="419" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C419" s="22"/>
     </row>
-    <row r="420" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="420" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C420" s="22"/>
     </row>
-    <row r="421" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="421" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C421" s="22"/>
     </row>
-    <row r="422" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="422" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C422" s="22"/>
     </row>
-    <row r="423" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="423" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C423" s="22"/>
     </row>
-    <row r="424" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="424" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C424" s="22"/>
     </row>
-    <row r="425" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="425" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C425" s="22"/>
     </row>
-    <row r="426" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="426" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C426" s="22"/>
     </row>
-    <row r="427" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="427" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C427" s="22"/>
     </row>
-    <row r="428" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="428" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C428" s="22"/>
     </row>
-    <row r="429" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="429" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C429" s="22"/>
     </row>
-    <row r="430" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="430" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C430" s="22"/>
     </row>
-    <row r="431" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="431" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C431" s="22"/>
     </row>
-    <row r="432" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="432" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C432" s="22"/>
     </row>
-    <row r="433" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="433" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C433" s="22"/>
     </row>
-    <row r="434" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="434" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C434" s="22"/>
     </row>
-    <row r="435" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="435" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C435" s="22"/>
     </row>
-    <row r="436" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="436" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C436" s="22"/>
     </row>
-    <row r="437" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="437" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C437" s="22"/>
     </row>
-    <row r="438" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="438" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C438" s="22"/>
     </row>
-    <row r="439" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="439" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C439" s="22"/>
     </row>
-    <row r="440" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="440" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C440" s="22"/>
     </row>
-    <row r="441" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="441" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C441" s="22"/>
     </row>
-    <row r="442" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="442" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C442" s="22"/>
     </row>
-    <row r="443" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="443" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C443" s="22"/>
     </row>
-    <row r="444" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="444" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C444" s="22"/>
     </row>
-    <row r="445" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="445" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C445" s="22"/>
     </row>
-    <row r="446" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="446" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C446" s="22"/>
     </row>
-    <row r="447" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="447" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C447" s="22"/>
     </row>
-    <row r="448" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="448" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C448" s="22"/>
     </row>
-    <row r="449" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="449" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C449" s="22"/>
     </row>
-    <row r="450" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="450" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C450" s="22"/>
     </row>
-    <row r="451" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="451" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C451" s="22"/>
     </row>
-    <row r="452" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="452" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C452" s="22"/>
     </row>
-    <row r="453" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="453" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C453" s="22"/>
     </row>
-    <row r="454" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="454" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C454" s="22"/>
     </row>
-    <row r="455" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="455" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C455" s="22"/>
     </row>
-    <row r="456" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="456" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C456" s="22"/>
     </row>
-    <row r="457" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="457" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C457" s="22"/>
     </row>
-    <row r="458" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="458" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C458" s="22"/>
     </row>
-    <row r="459" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="459" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C459" s="22"/>
     </row>
-    <row r="460" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="460" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C460" s="22"/>
     </row>
-    <row r="461" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="461" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C461" s="22"/>
     </row>
-    <row r="462" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="462" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C462" s="22"/>
     </row>
-    <row r="463" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="463" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C463" s="22"/>
     </row>
-    <row r="464" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="464" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C464" s="22"/>
     </row>
-    <row r="465" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="465" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C465" s="22"/>
     </row>
-    <row r="466" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="466" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C466" s="22"/>
     </row>
-    <row r="467" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="467" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C467" s="22"/>
     </row>
-    <row r="468" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="468" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C468" s="22"/>
     </row>
-    <row r="469" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="469" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C469" s="22"/>
     </row>
-    <row r="470" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="470" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C470" s="22"/>
     </row>
-    <row r="471" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="471" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C471" s="22"/>
     </row>
-    <row r="472" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="472" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C472" s="22"/>
     </row>
-    <row r="473" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="473" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C473" s="22"/>
     </row>
-    <row r="474" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="474" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C474" s="22"/>
     </row>
-    <row r="475" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="475" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C475" s="22"/>
     </row>
-    <row r="476" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="476" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C476" s="22"/>
     </row>
-    <row r="477" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="477" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C477" s="22"/>
     </row>
-    <row r="478" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="478" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C478" s="22"/>
     </row>
-    <row r="479" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="479" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C479" s="22"/>
     </row>
-    <row r="480" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="480" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C480" s="22"/>
     </row>
-    <row r="481" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="481" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C481" s="22"/>
     </row>
-    <row r="482" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="482" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C482" s="22"/>
     </row>
-    <row r="483" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="483" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C483" s="22"/>
     </row>
-    <row r="484" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="484" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C484" s="22"/>
     </row>
-    <row r="485" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="485" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C485" s="22"/>
     </row>
-    <row r="486" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="486" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C486" s="22"/>
     </row>
-    <row r="487" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="487" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C487" s="22"/>
     </row>
-    <row r="488" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="488" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C488" s="22"/>
     </row>
-    <row r="489" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="489" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C489" s="22"/>
     </row>
-    <row r="490" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="490" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C490" s="22"/>
     </row>
-    <row r="491" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="491" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C491" s="22"/>
     </row>
-    <row r="492" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="492" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C492" s="22"/>
     </row>
-    <row r="493" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="493" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C493" s="22"/>
     </row>
-    <row r="494" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="494" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C494" s="22"/>
     </row>
-    <row r="495" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="495" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C495" s="22"/>
     </row>
-    <row r="496" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="496" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C496" s="22"/>
     </row>
-    <row r="497" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="497" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C497" s="22"/>
     </row>
-    <row r="498" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="498" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C498" s="22"/>
     </row>
-    <row r="499" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="499" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C499" s="22"/>
     </row>
-    <row r="500" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="500" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C500" s="22"/>
     </row>
-    <row r="501" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="501" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C501" s="22"/>
     </row>
-    <row r="502" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="502" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C502" s="22"/>
     </row>
-    <row r="503" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="503" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C503" s="22"/>
     </row>
-    <row r="504" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="504" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C504" s="22"/>
     </row>
-    <row r="505" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="505" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C505" s="22"/>
     </row>
-    <row r="506" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="506" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C506" s="22"/>
     </row>
-    <row r="507" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="507" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C507" s="22"/>
     </row>
-    <row r="508" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="508" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C508" s="22"/>
     </row>
-    <row r="509" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="509" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C509" s="22"/>
     </row>
-    <row r="510" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="510" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C510" s="22"/>
     </row>
-    <row r="511" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="511" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C511" s="22"/>
     </row>
-    <row r="512" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="512" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C512" s="22"/>
     </row>
-    <row r="513" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="513" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C513" s="22"/>
     </row>
-    <row r="514" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="514" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C514" s="22"/>
     </row>
-    <row r="515" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="515" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C515" s="22"/>
     </row>
-    <row r="516" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="516" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C516" s="22"/>
     </row>
-    <row r="517" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="517" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C517" s="22"/>
     </row>
-    <row r="518" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="518" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C518" s="22"/>
     </row>
-    <row r="519" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="519" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C519" s="22"/>
     </row>
-    <row r="520" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="520" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C520" s="22"/>
     </row>
-    <row r="521" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="521" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C521" s="22"/>
     </row>
-    <row r="522" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="522" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C522" s="22"/>
     </row>
-    <row r="523" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="523" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C523" s="22"/>
     </row>
-    <row r="524" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="524" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C524" s="22"/>
     </row>
-    <row r="525" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="525" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C525" s="22"/>
     </row>
-    <row r="526" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="526" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C526" s="22"/>
     </row>
-    <row r="527" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="527" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C527" s="22"/>
     </row>
-    <row r="528" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="528" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C528" s="22"/>
     </row>
-    <row r="529" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="529" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C529" s="22"/>
     </row>
-    <row r="530" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="530" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C530" s="22"/>
     </row>
-    <row r="531" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="531" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C531" s="22"/>
     </row>
-    <row r="532" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="532" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C532" s="22"/>
     </row>
-    <row r="533" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="533" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C533" s="22"/>
     </row>
-    <row r="534" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="534" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C534" s="22"/>
     </row>
-    <row r="535" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="535" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C535" s="22"/>
     </row>
-    <row r="536" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="536" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C536" s="22"/>
     </row>
-    <row r="537" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="537" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C537" s="22"/>
     </row>
-    <row r="538" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="538" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C538" s="22"/>
     </row>
-    <row r="539" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="539" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C539" s="22"/>
     </row>
-    <row r="540" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="540" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C540" s="22"/>
     </row>
-    <row r="541" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="541" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C541" s="22"/>
     </row>
-    <row r="542" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="542" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C542" s="22"/>
     </row>
-    <row r="543" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="543" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C543" s="22"/>
     </row>
-    <row r="544" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="544" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C544" s="22"/>
     </row>
-    <row r="545" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="545" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C545" s="22"/>
     </row>
-    <row r="546" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="546" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C546" s="22"/>
     </row>
-    <row r="547" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="547" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C547" s="22"/>
     </row>
-    <row r="548" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="548" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C548" s="22"/>
     </row>
-    <row r="549" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="549" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C549" s="22"/>
     </row>
-    <row r="550" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="550" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C550" s="22"/>
     </row>
-    <row r="551" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="551" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C551" s="22"/>
     </row>
-    <row r="552" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="552" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C552" s="22"/>
     </row>
-    <row r="553" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="553" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C553" s="22"/>
     </row>
-    <row r="554" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="554" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C554" s="22"/>
     </row>
-    <row r="555" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="555" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C555" s="22"/>
     </row>
-    <row r="556" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="556" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C556" s="22"/>
     </row>
-    <row r="557" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="557" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C557" s="22"/>
     </row>
-    <row r="558" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="558" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C558" s="22"/>
     </row>
-    <row r="559" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="559" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C559" s="22"/>
     </row>
-    <row r="560" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="560" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C560" s="22"/>
     </row>
-    <row r="561" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="561" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C561" s="22"/>
     </row>
-    <row r="562" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="562" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C562" s="22"/>
     </row>
-    <row r="563" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="563" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C563" s="22"/>
     </row>
-    <row r="564" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="564" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C564" s="22"/>
     </row>
-    <row r="565" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="565" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C565" s="22"/>
     </row>
-    <row r="566" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="566" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C566" s="22"/>
     </row>
-    <row r="567" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="567" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C567" s="22"/>
     </row>
-    <row r="568" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="568" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C568" s="22"/>
     </row>
-    <row r="569" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="569" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C569" s="22"/>
     </row>
-    <row r="570" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="570" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C570" s="22"/>
     </row>
-    <row r="571" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="571" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C571" s="22"/>
     </row>
-    <row r="572" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="572" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C572" s="22"/>
     </row>
-    <row r="573" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="573" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C573" s="22"/>
     </row>
-    <row r="574" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="574" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C574" s="22"/>
     </row>
-    <row r="575" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="575" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C575" s="22"/>
     </row>
-    <row r="576" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="576" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C576" s="22"/>
     </row>
-    <row r="577" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="577" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C577" s="22"/>
     </row>
-    <row r="578" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="578" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C578" s="22"/>
     </row>
-    <row r="579" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="579" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C579" s="22"/>
     </row>
-    <row r="580" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="580" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C580" s="22"/>
     </row>
-    <row r="581" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="581" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C581" s="22"/>
     </row>
-    <row r="582" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="582" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C582" s="22"/>
     </row>
-    <row r="583" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="583" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C583" s="22"/>
     </row>
-    <row r="584" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="584" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C584" s="22"/>
     </row>
-    <row r="585" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="585" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C585" s="22"/>
     </row>
-    <row r="586" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="586" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C586" s="22"/>
     </row>
-    <row r="587" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="587" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C587" s="22"/>
     </row>
-    <row r="588" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="588" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C588" s="22"/>
     </row>
-    <row r="589" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="589" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C589" s="22"/>
     </row>
-    <row r="590" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="590" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C590" s="22"/>
     </row>
-    <row r="591" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="591" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C591" s="22"/>
     </row>
-    <row r="592" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="592" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C592" s="22"/>
     </row>
-    <row r="593" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="593" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C593" s="22"/>
     </row>
-    <row r="594" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="594" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C594" s="22"/>
     </row>
-    <row r="595" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="595" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C595" s="22"/>
     </row>
-    <row r="596" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="596" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C596" s="22"/>
     </row>
-    <row r="597" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="597" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C597" s="22"/>
     </row>
-    <row r="598" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="598" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C598" s="22"/>
     </row>
-    <row r="599" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="599" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C599" s="22"/>
     </row>
-    <row r="600" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="600" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C600" s="22"/>
     </row>
-    <row r="601" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="601" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C601" s="22"/>
     </row>
-    <row r="602" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="602" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C602" s="22"/>
     </row>
-    <row r="603" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="603" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C603" s="22"/>
     </row>
-    <row r="604" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="604" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C604" s="22"/>
     </row>
-    <row r="605" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="605" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C605" s="22"/>
     </row>
-    <row r="606" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="606" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C606" s="22"/>
     </row>
-    <row r="607" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="607" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C607" s="22"/>
     </row>
-    <row r="608" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="608" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C608" s="22"/>
     </row>
-    <row r="609" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="609" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C609" s="22"/>
     </row>
-    <row r="610" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="610" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C610" s="22"/>
     </row>
-    <row r="611" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="611" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C611" s="22"/>
     </row>
-    <row r="612" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="612" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C612" s="22"/>
     </row>
-    <row r="613" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="613" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C613" s="22"/>
     </row>
-    <row r="614" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="614" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C614" s="22"/>
     </row>
-    <row r="615" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="615" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C615" s="22"/>
     </row>
-    <row r="616" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="616" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C616" s="22"/>
     </row>
-    <row r="617" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="617" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C617" s="22"/>
     </row>
-    <row r="618" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="618" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C618" s="22"/>
     </row>
-    <row r="619" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="619" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C619" s="22"/>
     </row>
-    <row r="620" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="620" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C620" s="22"/>
     </row>
-    <row r="621" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="621" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C621" s="22"/>
     </row>
-    <row r="622" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="622" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C622" s="22"/>
     </row>
-    <row r="623" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="623" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C623" s="22"/>
     </row>
-    <row r="624" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="624" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C624" s="22"/>
     </row>
-    <row r="625" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="625" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C625" s="22"/>
     </row>
-    <row r="626" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="626" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C626" s="22"/>
     </row>
-    <row r="627" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="627" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C627" s="22"/>
     </row>
-    <row r="628" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="628" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C628" s="22"/>
     </row>
-    <row r="629" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="629" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C629" s="22"/>
     </row>
-    <row r="630" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="630" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C630" s="22"/>
     </row>
-    <row r="631" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="631" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C631" s="22"/>
     </row>
-    <row r="632" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="632" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C632" s="22"/>
     </row>
-    <row r="633" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="633" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C633" s="22"/>
     </row>
-    <row r="634" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="634" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C634" s="22"/>
     </row>
-    <row r="635" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="635" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C635" s="22"/>
     </row>
-    <row r="636" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="636" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C636" s="22"/>
     </row>
-    <row r="637" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="637" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C637" s="22"/>
     </row>
-    <row r="638" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="638" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C638" s="22"/>
     </row>
-    <row r="639" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="639" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C639" s="22"/>
     </row>
-    <row r="640" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="640" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C640" s="22"/>
     </row>
-    <row r="641" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="641" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C641" s="22"/>
     </row>
-    <row r="642" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="642" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C642" s="22"/>
     </row>
-    <row r="643" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="643" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C643" s="22"/>
     </row>
-    <row r="644" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="644" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C644" s="22"/>
     </row>
-    <row r="645" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="645" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C645" s="22"/>
     </row>
-    <row r="646" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="646" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C646" s="22"/>
     </row>
-    <row r="647" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="647" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C647" s="22"/>
     </row>
-    <row r="648" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="648" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C648" s="22"/>
     </row>
-    <row r="649" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="649" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C649" s="22"/>
     </row>
-    <row r="650" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="650" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C650" s="22"/>
     </row>
-    <row r="651" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="651" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C651" s="22"/>
     </row>
-    <row r="652" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="652" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C652" s="22"/>
     </row>
-    <row r="653" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="653" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C653" s="22"/>
     </row>
-    <row r="654" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="654" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C654" s="22"/>
     </row>
-    <row r="655" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="655" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C655" s="22"/>
     </row>
-    <row r="656" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="656" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C656" s="22"/>
     </row>
-    <row r="657" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="657" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C657" s="22"/>
     </row>
-    <row r="658" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="658" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C658" s="22"/>
     </row>
-    <row r="659" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="659" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C659" s="22"/>
     </row>
-    <row r="660" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="660" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C660" s="22"/>
     </row>
-    <row r="661" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="661" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C661" s="22"/>
     </row>
-    <row r="662" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="662" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C662" s="22"/>
     </row>
-    <row r="663" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="663" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C663" s="22"/>
     </row>
-    <row r="664" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="664" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C664" s="22"/>
     </row>
-    <row r="665" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="665" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C665" s="22"/>
     </row>
-    <row r="666" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="666" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C666" s="22"/>
     </row>
-    <row r="667" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="667" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C667" s="22"/>
     </row>
-    <row r="668" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="668" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C668" s="22"/>
     </row>
-    <row r="669" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="669" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C669" s="22"/>
     </row>
-    <row r="670" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="670" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C670" s="22"/>
     </row>
-    <row r="671" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="671" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C671" s="22"/>
     </row>
-    <row r="672" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="672" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C672" s="22"/>
     </row>
-    <row r="673" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="673" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C673" s="22"/>
     </row>
-    <row r="674" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="674" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C674" s="22"/>
     </row>
-    <row r="675" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="675" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C675" s="22"/>
     </row>
-    <row r="676" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="676" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C676" s="22"/>
     </row>
-    <row r="677" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="677" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C677" s="22"/>
     </row>
-    <row r="678" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="678" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C678" s="22"/>
     </row>
-    <row r="679" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="679" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C679" s="22"/>
     </row>
-    <row r="680" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="680" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C680" s="22"/>
     </row>
-    <row r="681" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="681" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C681" s="22"/>
     </row>
-    <row r="682" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="682" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C682" s="22"/>
     </row>
-    <row r="683" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="683" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C683" s="22"/>
     </row>
-    <row r="684" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="684" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C684" s="22"/>
     </row>
-    <row r="685" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="685" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C685" s="22"/>
     </row>
-    <row r="686" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="686" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C686" s="22"/>
     </row>
-    <row r="687" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="687" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C687" s="22"/>
     </row>
-    <row r="688" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="688" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C688" s="22"/>
     </row>
-    <row r="689" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="689" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C689" s="22"/>
     </row>
-    <row r="690" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="690" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C690" s="22"/>
     </row>
-    <row r="691" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="691" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C691" s="22"/>
     </row>
-    <row r="692" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="692" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C692" s="22"/>
     </row>
-    <row r="693" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="693" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C693" s="22"/>
     </row>
-    <row r="694" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="694" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C694" s="22"/>
     </row>
-    <row r="695" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="695" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C695" s="22"/>
     </row>
-    <row r="696" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="696" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C696" s="22"/>
     </row>
-    <row r="697" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="697" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C697" s="22"/>
     </row>
-    <row r="698" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="698" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C698" s="22"/>
     </row>
-    <row r="699" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="699" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C699" s="22"/>
     </row>
-    <row r="700" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="700" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C700" s="22"/>
     </row>
-    <row r="701" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="701" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C701" s="22"/>
     </row>
-    <row r="702" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="702" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C702" s="22"/>
     </row>
-    <row r="703" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="703" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C703" s="22"/>
     </row>
-    <row r="704" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="704" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C704" s="22"/>
     </row>
-    <row r="705" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="705" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C705" s="22"/>
     </row>
-    <row r="706" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="706" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C706" s="22"/>
     </row>
-    <row r="707" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="707" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C707" s="22"/>
     </row>
-    <row r="708" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="708" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C708" s="22"/>
     </row>
-    <row r="709" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="709" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C709" s="22"/>
     </row>
-    <row r="710" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="710" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C710" s="22"/>
     </row>
-    <row r="711" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="711" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C711" s="22"/>
     </row>
-    <row r="712" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="712" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C712" s="22"/>
     </row>
-    <row r="713" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="713" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C713" s="22"/>
     </row>
-    <row r="714" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="714" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C714" s="22"/>
     </row>
-    <row r="715" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="715" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C715" s="22"/>
     </row>
-    <row r="716" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="716" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C716" s="22"/>
     </row>
-    <row r="717" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="717" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C717" s="22"/>
     </row>
-    <row r="718" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="718" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C718" s="22"/>
     </row>
-    <row r="719" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="719" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C719" s="22"/>
     </row>
-    <row r="720" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="720" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C720" s="22"/>
     </row>
-    <row r="721" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="721" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C721" s="22"/>
     </row>
-    <row r="722" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="722" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C722" s="22"/>
     </row>
-    <row r="723" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="723" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C723" s="22"/>
     </row>
-    <row r="724" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="724" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C724" s="22"/>
     </row>
-    <row r="725" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="725" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C725" s="22"/>
     </row>
-    <row r="726" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="726" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C726" s="22"/>
     </row>
-    <row r="727" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="727" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C727" s="22"/>
     </row>
-    <row r="728" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="728" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C728" s="22"/>
     </row>
-    <row r="729" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="729" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C729" s="22"/>
     </row>
-    <row r="730" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="730" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C730" s="22"/>
     </row>
-    <row r="731" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="731" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C731" s="22"/>
     </row>
-    <row r="732" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="732" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C732" s="22"/>
     </row>
-    <row r="733" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="733" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C733" s="22"/>
     </row>
-    <row r="734" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="734" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C734" s="22"/>
     </row>
-    <row r="735" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="735" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C735" s="22"/>
     </row>
-    <row r="736" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="736" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C736" s="22"/>
     </row>
-    <row r="737" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="737" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C737" s="22"/>
     </row>
-    <row r="738" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="738" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C738" s="22"/>
     </row>
-    <row r="739" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="739" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C739" s="22"/>
     </row>
-    <row r="740" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="740" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C740" s="22"/>
     </row>
-    <row r="741" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="741" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C741" s="22"/>
     </row>
-    <row r="742" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="742" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C742" s="22"/>
     </row>
-    <row r="743" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="743" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C743" s="22"/>
     </row>
-    <row r="744" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="744" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C744" s="22"/>
     </row>
-    <row r="745" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="745" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C745" s="22"/>
     </row>
-    <row r="746" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="746" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C746" s="22"/>
     </row>
-    <row r="747" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="747" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C747" s="22"/>
     </row>
-    <row r="748" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="748" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C748" s="22"/>
     </row>
-    <row r="749" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="749" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C749" s="22"/>
     </row>
-    <row r="750" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="750" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C750" s="22"/>
     </row>
-    <row r="751" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="751" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C751" s="22"/>
     </row>
-    <row r="752" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="752" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C752" s="22"/>
     </row>
-    <row r="753" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="753" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C753" s="22"/>
     </row>
-    <row r="754" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="754" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C754" s="22"/>
     </row>
-    <row r="755" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="755" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C755" s="22"/>
     </row>
-    <row r="756" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="756" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C756" s="22"/>
     </row>
-    <row r="757" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="757" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C757" s="22"/>
     </row>
-    <row r="758" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="758" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C758" s="22"/>
     </row>
-    <row r="759" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="759" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C759" s="22"/>
     </row>
-    <row r="760" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="760" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C760" s="22"/>
     </row>
-    <row r="761" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="761" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C761" s="22"/>
     </row>
-    <row r="762" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="762" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C762" s="22"/>
     </row>
-    <row r="763" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="763" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C763" s="22"/>
     </row>
-    <row r="764" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="764" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C764" s="22"/>
     </row>
-    <row r="765" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="765" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C765" s="22"/>
     </row>
-    <row r="766" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="766" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C766" s="22"/>
     </row>
-    <row r="767" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="767" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C767" s="22"/>
     </row>
-    <row r="768" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="768" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C768" s="22"/>
     </row>
-    <row r="769" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="769" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C769" s="22"/>
     </row>
-    <row r="770" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="770" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C770" s="22"/>
     </row>
-    <row r="771" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="771" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C771" s="22"/>
     </row>
-    <row r="772" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="772" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C772" s="22"/>
     </row>
-    <row r="773" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="773" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C773" s="22"/>
     </row>
-    <row r="774" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="774" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C774" s="22"/>
     </row>
-    <row r="775" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="775" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C775" s="22"/>
     </row>
-    <row r="776" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="776" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C776" s="22"/>
     </row>
-    <row r="777" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="777" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C777" s="22"/>
     </row>
-    <row r="778" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="778" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C778" s="22"/>
     </row>
-    <row r="779" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="779" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C779" s="22"/>
     </row>
-    <row r="780" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="780" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C780" s="22"/>
     </row>
-    <row r="781" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="781" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C781" s="22"/>
     </row>
-    <row r="782" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="782" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C782" s="22"/>
     </row>
-    <row r="783" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="783" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C783" s="22"/>
     </row>
-    <row r="784" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="784" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C784" s="22"/>
     </row>
-    <row r="785" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="785" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C785" s="22"/>
     </row>
-    <row r="786" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="786" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C786" s="22"/>
     </row>
-    <row r="787" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="787" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C787" s="22"/>
     </row>
-    <row r="788" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="788" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C788" s="22"/>
     </row>
-    <row r="789" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="789" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C789" s="22"/>
     </row>
-    <row r="790" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="790" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C790" s="22"/>
     </row>
-    <row r="791" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="791" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C791" s="22"/>
     </row>
-    <row r="792" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="792" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C792" s="22"/>
     </row>
-    <row r="793" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="793" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C793" s="22"/>
     </row>
-    <row r="794" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="794" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C794" s="22"/>
     </row>
-    <row r="795" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="795" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C795" s="22"/>
     </row>
-    <row r="796" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="796" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C796" s="22"/>
     </row>
-    <row r="797" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="797" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C797" s="22"/>
     </row>
-    <row r="798" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="798" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C798" s="22"/>
     </row>
-    <row r="799" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="799" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C799" s="22"/>
     </row>
-    <row r="800" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="800" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C800" s="22"/>
     </row>
-    <row r="801" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="801" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C801" s="22"/>
     </row>
-    <row r="802" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="802" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C802" s="22"/>
     </row>
-    <row r="803" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="803" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C803" s="22"/>
     </row>
-    <row r="804" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="804" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C804" s="22"/>
     </row>
-    <row r="805" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="805" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C805" s="22"/>
     </row>
-    <row r="806" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="806" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C806" s="22"/>
     </row>
-    <row r="807" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="807" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C807" s="22"/>
     </row>
-    <row r="808" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="808" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C808" s="22"/>
     </row>
-    <row r="809" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="809" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C809" s="22"/>
     </row>
-    <row r="810" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="810" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C810" s="22"/>
     </row>
-    <row r="811" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="811" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C811" s="22"/>
     </row>
-    <row r="812" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="812" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C812" s="22"/>
     </row>
-    <row r="813" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="813" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C813" s="22"/>
     </row>
-    <row r="814" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="814" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C814" s="22"/>
     </row>
-    <row r="815" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="815" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C815" s="22"/>
     </row>
-    <row r="816" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="816" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C816" s="22"/>
     </row>
-    <row r="817" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="817" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C817" s="22"/>
     </row>
-    <row r="818" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="818" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C818" s="22"/>
     </row>
-    <row r="819" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="819" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C819" s="22"/>
     </row>
-    <row r="820" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="820" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C820" s="22"/>
     </row>
-    <row r="821" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="821" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C821" s="22"/>
     </row>
-    <row r="822" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="822" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C822" s="22"/>
     </row>
-    <row r="823" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="823" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C823" s="22"/>
     </row>
-    <row r="824" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="824" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C824" s="22"/>
     </row>
-    <row r="825" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="825" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C825" s="22"/>
     </row>
-    <row r="826" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="826" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C826" s="22"/>
     </row>
-    <row r="827" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="827" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C827" s="22"/>
     </row>
-    <row r="828" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="828" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C828" s="22"/>
     </row>
-    <row r="829" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="829" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C829" s="22"/>
     </row>
-    <row r="830" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="830" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C830" s="22"/>
     </row>
-    <row r="831" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="831" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C831" s="22"/>
     </row>
-    <row r="832" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="832" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C832" s="22"/>
     </row>
-    <row r="833" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="833" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C833" s="22"/>
     </row>
-    <row r="834" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="834" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C834" s="22"/>
     </row>
-    <row r="835" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="835" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C835" s="22"/>
     </row>
-    <row r="836" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="836" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C836" s="22"/>
     </row>
-    <row r="837" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="837" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C837" s="22"/>
     </row>
-    <row r="838" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="838" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C838" s="22"/>
     </row>
-    <row r="839" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="839" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C839" s="22"/>
     </row>
-    <row r="840" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="840" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C840" s="22"/>
     </row>
-    <row r="841" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="841" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C841" s="22"/>
     </row>
-    <row r="842" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="842" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C842" s="22"/>
     </row>
-    <row r="843" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="843" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C843" s="22"/>
     </row>
-    <row r="844" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="844" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C844" s="22"/>
     </row>
-    <row r="845" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="845" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C845" s="22"/>
     </row>
-    <row r="846" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="846" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C846" s="22"/>
     </row>
-    <row r="847" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="847" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C847" s="22"/>
     </row>
-    <row r="848" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="848" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C848" s="22"/>
     </row>
-    <row r="849" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="849" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C849" s="22"/>
     </row>
-    <row r="850" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="850" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C850" s="22"/>
     </row>
-    <row r="851" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="851" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C851" s="22"/>
     </row>
-    <row r="852" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="852" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C852" s="22"/>
     </row>
-    <row r="853" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="853" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C853" s="22"/>
     </row>
-    <row r="854" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="854" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C854" s="22"/>
     </row>
-    <row r="855" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="855" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C855" s="22"/>
     </row>
-    <row r="856" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="856" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C856" s="22"/>
     </row>
-    <row r="857" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="857" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C857" s="22"/>
     </row>
-    <row r="858" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="858" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C858" s="22"/>
     </row>
-    <row r="859" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="859" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C859" s="22"/>
     </row>
-    <row r="860" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="860" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C860" s="22"/>
     </row>
-    <row r="861" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="861" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C861" s="22"/>
     </row>
-    <row r="862" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="862" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C862" s="22"/>
     </row>
-    <row r="863" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="863" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C863" s="22"/>
     </row>
-    <row r="864" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="864" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C864" s="22"/>
     </row>
-    <row r="865" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="865" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C865" s="22"/>
     </row>
-    <row r="866" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="866" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C866" s="22"/>
     </row>
-    <row r="867" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="867" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C867" s="22"/>
     </row>
-    <row r="868" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="868" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C868" s="22"/>
     </row>
-    <row r="869" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="869" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C869" s="22"/>
     </row>
-    <row r="870" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="870" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C870" s="22"/>
     </row>
-    <row r="871" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="871" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C871" s="22"/>
     </row>
-    <row r="872" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="872" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C872" s="22"/>
     </row>
-    <row r="873" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="873" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C873" s="22"/>
     </row>
-    <row r="874" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="874" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C874" s="22"/>
     </row>
-    <row r="875" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="875" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C875" s="22"/>
     </row>
-    <row r="876" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="876" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C876" s="22"/>
     </row>
-    <row r="877" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="877" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C877" s="22"/>
     </row>
-    <row r="878" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="878" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C878" s="22"/>
     </row>
-    <row r="879" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="879" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C879" s="22"/>
     </row>
-    <row r="880" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="880" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C880" s="22"/>
     </row>
-    <row r="881" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="881" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C881" s="22"/>
     </row>
-    <row r="882" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="882" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C882" s="22"/>
     </row>
-    <row r="883" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="883" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C883" s="22"/>
     </row>
-    <row r="884" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="884" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C884" s="22"/>
     </row>
-    <row r="885" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="885" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C885" s="22"/>
     </row>
-    <row r="886" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="886" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C886" s="22"/>
     </row>
-    <row r="887" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="887" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C887" s="22"/>
     </row>
-    <row r="888" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="888" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C888" s="22"/>
     </row>
-    <row r="889" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="889" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C889" s="22"/>
     </row>
-    <row r="890" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="890" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C890" s="22"/>
     </row>
-    <row r="891" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="891" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C891" s="22"/>
     </row>
-    <row r="892" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="892" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C892" s="22"/>
     </row>
-    <row r="893" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="893" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C893" s="22"/>
     </row>
-    <row r="894" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="894" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C894" s="22"/>
     </row>
-    <row r="895" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="895" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C895" s="22"/>
     </row>
-    <row r="896" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="896" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C896" s="22"/>
     </row>
-    <row r="897" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="897" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C897" s="22"/>
     </row>
-    <row r="898" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="898" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C898" s="22"/>
     </row>
-    <row r="899" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="899" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C899" s="22"/>
     </row>
-    <row r="900" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="900" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C900" s="22"/>
     </row>
-    <row r="901" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="901" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C901" s="22"/>
     </row>
-    <row r="902" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="902" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C902" s="22"/>
     </row>
-    <row r="903" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="903" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C903" s="22"/>
     </row>
-    <row r="904" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="904" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C904" s="22"/>
     </row>
-    <row r="905" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="905" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C905" s="22"/>
     </row>
-    <row r="906" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="906" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C906" s="22"/>
     </row>
-    <row r="907" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="907" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C907" s="22"/>
     </row>
-    <row r="908" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="908" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C908" s="22"/>
     </row>
-    <row r="909" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="909" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C909" s="22"/>
     </row>
-    <row r="910" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="910" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C910" s="22"/>
     </row>
-    <row r="911" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="911" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C911" s="22"/>
     </row>
-    <row r="912" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="912" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C912" s="22"/>
     </row>
-    <row r="913" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="913" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C913" s="22"/>
     </row>
-    <row r="914" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="914" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C914" s="22"/>
     </row>
-    <row r="915" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="915" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C915" s="22"/>
     </row>
-    <row r="916" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="916" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C916" s="22"/>
     </row>
-    <row r="917" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="917" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C917" s="22"/>
     </row>
-    <row r="918" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="918" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C918" s="22"/>
     </row>
-    <row r="919" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="919" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C919" s="22"/>
     </row>
-    <row r="920" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="920" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C920" s="22"/>
     </row>
-    <row r="921" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="921" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C921" s="22"/>
     </row>
-    <row r="922" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="922" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C922" s="22"/>
     </row>
-    <row r="923" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="923" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C923" s="22"/>
     </row>
-    <row r="924" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="924" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C924" s="22"/>
     </row>
-    <row r="925" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="925" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C925" s="22"/>
     </row>
-    <row r="926" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="926" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C926" s="22"/>
     </row>
-    <row r="927" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="927" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C927" s="22"/>
     </row>
-    <row r="928" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="928" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C928" s="22"/>
     </row>
-    <row r="929" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="929" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C929" s="22"/>
     </row>
-    <row r="930" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="930" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C930" s="22"/>
     </row>
-    <row r="931" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="931" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C931" s="22"/>
     </row>
-    <row r="932" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="932" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C932" s="22"/>
     </row>
-    <row r="933" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="933" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C933" s="22"/>
     </row>
-    <row r="934" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="934" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C934" s="22"/>
     </row>
-    <row r="935" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="935" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C935" s="22"/>
     </row>
-    <row r="936" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="936" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C936" s="22"/>
     </row>
-    <row r="937" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="937" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C937" s="22"/>
     </row>
-    <row r="938" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="938" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C938" s="22"/>
     </row>
-    <row r="939" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="939" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C939" s="22"/>
     </row>
-    <row r="940" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="940" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C940" s="22"/>
     </row>
-    <row r="941" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="941" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C941" s="22"/>
     </row>
-    <row r="942" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="942" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C942" s="22"/>
     </row>
-    <row r="943" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="943" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C943" s="22"/>
     </row>
-    <row r="944" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="944" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C944" s="22"/>
     </row>
-    <row r="945" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="945" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C945" s="22"/>
     </row>
-    <row r="946" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="946" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C946" s="22"/>
     </row>
-    <row r="947" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="947" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C947" s="22"/>
     </row>
-    <row r="948" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="948" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C948" s="22"/>
     </row>
-    <row r="949" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="949" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C949" s="22"/>
     </row>
-    <row r="950" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="950" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C950" s="22"/>
     </row>
-    <row r="951" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="951" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C951" s="22"/>
     </row>
-    <row r="952" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="952" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C952" s="22"/>
     </row>
-    <row r="953" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="953" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C953" s="22"/>
     </row>
-    <row r="954" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="954" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C954" s="22"/>
     </row>
-    <row r="955" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="955" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C955" s="22"/>
     </row>
-    <row r="956" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="956" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C956" s="22"/>
     </row>
-    <row r="957" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="957" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C957" s="22"/>
     </row>
-    <row r="958" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="958" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C958" s="22"/>
     </row>
-    <row r="959" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="959" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C959" s="22"/>
     </row>
-    <row r="960" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="960" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C960" s="22"/>
     </row>
-    <row r="961" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="961" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C961" s="22"/>
     </row>
-    <row r="962" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="962" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C962" s="22"/>
     </row>
-    <row r="963" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="963" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C963" s="22"/>
     </row>
-    <row r="964" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="964" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C964" s="22"/>
     </row>
-    <row r="965" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="965" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C965" s="22"/>
     </row>
-    <row r="966" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="966" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C966" s="22"/>
     </row>
-    <row r="967" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="967" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C967" s="22"/>
     </row>
-    <row r="968" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="968" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C968" s="22"/>
     </row>
-    <row r="969" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="969" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C969" s="22"/>
     </row>
-    <row r="970" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="970" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C970" s="22"/>
     </row>
-    <row r="971" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="971" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C971" s="22"/>
     </row>
-    <row r="972" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="972" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C972" s="22"/>
     </row>
-    <row r="973" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="973" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C973" s="22"/>
     </row>
-    <row r="974" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="974" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C974" s="22"/>
     </row>
-    <row r="975" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="975" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C975" s="22"/>
     </row>
-    <row r="976" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="976" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C976" s="22"/>
     </row>
-    <row r="977" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="977" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C977" s="22"/>
     </row>
-    <row r="978" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="978" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C978" s="22"/>
     </row>
-    <row r="979" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="979" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C979" s="22"/>
     </row>
-    <row r="980" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="980" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C980" s="22"/>
     </row>
-    <row r="981" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="981" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C981" s="22"/>
     </row>
-    <row r="982" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="982" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C982" s="22"/>
     </row>
-    <row r="983" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="983" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C983" s="22"/>
     </row>
-    <row r="984" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="984" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C984" s="22"/>
     </row>
-    <row r="985" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="985" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C985" s="22"/>
     </row>
-    <row r="986" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="986" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C986" s="22"/>
     </row>
-    <row r="987" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="987" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C987" s="22"/>
     </row>
-    <row r="988" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="988" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C988" s="22"/>
     </row>
-    <row r="989" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="989" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C989" s="22"/>
     </row>
-    <row r="990" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="990" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C990" s="22"/>
     </row>
-    <row r="991" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="991" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C991" s="22"/>
     </row>
-    <row r="992" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="992" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C992" s="22"/>
     </row>
-    <row r="993" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="993" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C993" s="22"/>
     </row>
-    <row r="994" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="994" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C994" s="22"/>
     </row>
-    <row r="995" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="995" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C995" s="22"/>
     </row>
-    <row r="996" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="996" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C996" s="22"/>
     </row>
-    <row r="997" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="997" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C997" s="22"/>
     </row>
-    <row r="998" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="998" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C998" s="22"/>
     </row>
-    <row r="999" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="999" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C999" s="22"/>
     </row>
-    <row r="1000" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1000" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1000" s="22"/>
     </row>
   </sheetData>

</xml_diff>